<commit_message>
removed questions without links
</commit_message>
<xml_diff>
--- a/data/chatbot-1.xlsx
+++ b/data/chatbot-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJK3794\PycharmProjects\Datahub Chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49092F73-4EDF-4FCC-8C30-2E3E68091264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5AAF31-3EA6-44E3-8F5A-6B63211D08FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{CB1DE796-0A7F-4358-B0F5-62D7433C0693}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="400">
   <si>
     <t>Category</t>
   </si>
@@ -995,9 +995,6 @@
     <t>What is the current MDLZ- Azure HLD set up ?</t>
   </si>
   <si>
-    <t>What are the best practices related to Azure and Databricks services?</t>
-  </si>
-  <si>
     <t>What services does the data integration tower provide?</t>
   </si>
   <si>
@@ -1010,9 +1007,6 @@
     <t>How to raise a servicenow ticket for Alteryx?</t>
   </si>
   <si>
-    <t>How can I create custom reports and visualizations from Alteryx workflows?</t>
-  </si>
-  <si>
     <t>Are there any training documents for Alteryx?</t>
   </si>
   <si>
@@ -1025,30 +1019,12 @@
     <t>Who should I contact if my data integration job in Aecorsoft fails?</t>
   </si>
   <si>
-    <t>How do I request access to specific data sets or reports through Collibra?</t>
-  </si>
-  <si>
-    <t>How can I use Collibra to check the quality of data I’m working with?</t>
-  </si>
-  <si>
     <t>What tools and services are offered under SAP BI services?</t>
   </si>
   <si>
-    <t>Where can I find documents related to SAP BI reporting and analytics?</t>
-  </si>
-  <si>
-    <t>How can I access support resources for SAP BI?</t>
-  </si>
-  <si>
     <t>Who do I reach out to incase I need any support?</t>
   </si>
   <si>
-    <t>How do I raise a support ticket for issues related to the D&amp;A platform?</t>
-  </si>
-  <si>
-    <t>How can I request access to specific D&amp;A platform environments?</t>
-  </si>
-  <si>
     <t>Where can I find information on pre-production environment?</t>
   </si>
   <si>
@@ -1146,9 +1122,6 @@
   </si>
   <si>
     <t>https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Pre%20Prod%20Readiness.aspx?csf=1&amp;web=1&amp;e=kbE51k#expectation-from-product-teams</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>MDSDataAnalyticsPlatforms</t>
@@ -1712,11 +1685,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}">
-  <dimension ref="A1:L148"/>
+  <dimension ref="A1:L140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="87" zoomScaleNormal="72" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F130" sqref="F130"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B129" activeCellId="1" sqref="A134:XFD134 A129:XFD129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4022,67 +3995,67 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="C110" s="16" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D110" t="s">
         <v>298</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="C111" s="16" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D111" t="s">
         <v>299</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="F111" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="C112" s="16" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D112" t="s">
         <v>300</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="F112" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B113" s="16" t="s">
         <v>286</v>
@@ -4094,15 +4067,15 @@
         <v>301</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="F113" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B114" s="16" t="s">
         <v>286</v>
@@ -4114,15 +4087,15 @@
         <v>302</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="F114" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B115" s="16" t="s">
         <v>286</v>
@@ -4134,670 +4107,510 @@
         <v>303</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="F115" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B116" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="C116" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="D116" t="s">
         <v>304</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="F116" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B117" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C117" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D117" t="s">
         <v>305</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="F117" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B118" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C118" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D118" t="s">
         <v>306</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="F118" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B119" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C119" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D119" t="s">
         <v>307</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="F119" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B120" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C120" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D120" t="s">
         <v>308</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="F120" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B121" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="C121" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="D121" t="s">
         <v>309</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="F121" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B122" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="C122" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="D122" t="s">
         <v>310</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="F122" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B123" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="C123" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="D123" t="s">
         <v>311</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="F123" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B124" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="C124" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="D124" t="s">
         <v>312</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="F124" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B125" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="C125" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="D125" t="s">
         <v>313</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="F125" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B126" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="C126" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="D126" t="s">
         <v>314</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="F126" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B127" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="C127" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="D127" t="s">
         <v>315</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="F127" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B128" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="C128" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="D128" t="s">
         <v>316</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F128" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B129" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C129" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D129" t="s">
         <v>317</v>
       </c>
-      <c r="E129" t="s">
-        <v>368</v>
+      <c r="E129" s="1" t="s">
+        <v>348</v>
       </c>
       <c r="F129" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B130" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C130" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D130" t="s">
         <v>318</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="F130" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B131" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C131" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D131" t="s">
         <v>319</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="F131" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B132" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C132" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D132" t="s">
         <v>320</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="F132" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B133" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C133" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D133" t="s">
         <v>321</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="F133" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B134" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C134" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D134" t="s">
         <v>322</v>
       </c>
-      <c r="E134" t="s">
-        <v>368</v>
+      <c r="E134" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="F134" t="s">
-        <v>368</v>
+        <v>393</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B135" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C135" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D135" t="s">
         <v>323</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="F135" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B136" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C136" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D136" t="s">
         <v>324</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F136" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B137" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C137" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="D137" t="s">
         <v>325</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="F137" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B138" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C138" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D138" t="s">
         <v>326</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F138" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
+        <v>363</v>
+      </c>
+      <c r="B139" t="s">
         <v>372</v>
       </c>
-      <c r="B139" t="s">
-        <v>378</v>
-      </c>
       <c r="C139" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D139" t="s">
         <v>327</v>
       </c>
-      <c r="E139" t="s">
-        <v>368</v>
+      <c r="E139" s="1" t="s">
+        <v>358</v>
       </c>
       <c r="F139" t="s">
-        <v>368</v>
+        <v>398</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
+        <v>363</v>
+      </c>
+      <c r="B140" t="s">
         <v>372</v>
       </c>
-      <c r="B140" t="s">
-        <v>378</v>
-      </c>
       <c r="C140" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D140" t="s">
         <v>328</v>
       </c>
-      <c r="E140" t="s">
-        <v>368</v>
+      <c r="E140" s="1" t="s">
+        <v>359</v>
       </c>
       <c r="F140" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
-        <v>372</v>
-      </c>
-      <c r="B141" t="s">
-        <v>379</v>
-      </c>
-      <c r="C141" t="s">
-        <v>379</v>
-      </c>
-      <c r="D141" t="s">
-        <v>329</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="F141" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
-        <v>372</v>
-      </c>
-      <c r="B142" t="s">
-        <v>379</v>
-      </c>
-      <c r="C142" t="s">
-        <v>379</v>
-      </c>
-      <c r="D142" t="s">
-        <v>330</v>
-      </c>
-      <c r="E142" t="s">
-        <v>368</v>
-      </c>
-      <c r="F142" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
-        <v>372</v>
-      </c>
-      <c r="B143" t="s">
-        <v>379</v>
-      </c>
-      <c r="C143" t="s">
-        <v>379</v>
-      </c>
-      <c r="D143" t="s">
-        <v>331</v>
-      </c>
-      <c r="E143" t="s">
-        <v>368</v>
-      </c>
-      <c r="F143" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
-        <v>372</v>
-      </c>
-      <c r="B144" t="s">
-        <v>380</v>
-      </c>
-      <c r="C144" t="s">
-        <v>380</v>
-      </c>
-      <c r="D144" t="s">
-        <v>332</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="F144" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
-        <v>372</v>
-      </c>
-      <c r="B145" t="s">
-        <v>380</v>
-      </c>
-      <c r="C145" t="s">
-        <v>380</v>
-      </c>
-      <c r="D145" t="s">
-        <v>333</v>
-      </c>
-      <c r="E145" t="s">
-        <v>368</v>
-      </c>
-      <c r="F145" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
-        <v>372</v>
-      </c>
-      <c r="B146" t="s">
-        <v>380</v>
-      </c>
-      <c r="C146" t="s">
-        <v>380</v>
-      </c>
-      <c r="D146" t="s">
-        <v>334</v>
-      </c>
-      <c r="E146" t="s">
-        <v>368</v>
-      </c>
-      <c r="F146" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
-        <v>372</v>
-      </c>
-      <c r="B147" t="s">
-        <v>381</v>
-      </c>
-      <c r="C147" t="s">
-        <v>381</v>
-      </c>
-      <c r="D147" t="s">
-        <v>335</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="F147" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
-        <v>372</v>
-      </c>
-      <c r="B148" t="s">
-        <v>381</v>
-      </c>
-      <c r="C148" t="s">
-        <v>381</v>
-      </c>
-      <c r="D148" t="s">
-        <v>336</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="F148" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -5045,18 +4858,18 @@
     <hyperlink ref="E126" r:id="rId240" location="azure-cloud-platform" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Service-catalogue.aspx - azure-cloud-platform" xr:uid="{03EA318F-4F44-4564-BDB2-9B1BDB28E2CE}"/>
     <hyperlink ref="E127" r:id="rId241" display="https://collaboration.mdlz.com/:b:/r/sites/MDSDataAnalyticsPlatforms/Resources/Azure Platform/Databricks_Platform_Overview_0.2.pdf?csf=1&amp;web=1&amp;e=ztKvMt" xr:uid="{D66210B6-DE46-435B-9D50-0821EEF406A7}"/>
     <hyperlink ref="E128" r:id="rId242" display="https://collaboration.mdlz.com/:b:/r/sites/MDSDataAnalyticsPlatforms/Resources/Azure Platform/MDLZ-Azure-Design-Diagrams-V2 - Azure-HLD1.pdf?csf=1&amp;web=1&amp;e=JqdokL" xr:uid="{5F8FE5E4-3139-4DD4-912D-5554A2D3F484}"/>
-    <hyperlink ref="E130" r:id="rId243" location="data-integration-platforms" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Service-catalogue.aspx - data-integration-platforms" xr:uid="{DBCD28CC-93A8-4C9B-B4E9-44A5D42822E4}"/>
-    <hyperlink ref="E131" r:id="rId244" display="https://collaboration.mdlz.com/:b:/r/sites/alteryx/Shared Documents/Guidlines for Alteryx usage- MDLZ.pdf?csf=1&amp;web=1&amp;e=owyGdK" xr:uid="{13C082D6-C3B9-4755-A934-E699194D8CDE}"/>
-    <hyperlink ref="E132" r:id="rId245" display="https://collaboration.mdlz.com/:b:/r/sites/alteryx/Shared Documents/Alteryx New Project Setup %26 Best Practices.pdf?csf=1&amp;web=1&amp;e=2NAIcG" xr:uid="{4F8EA5C5-572E-45D0-8906-E57D0525F255}"/>
-    <hyperlink ref="E133" r:id="rId246" display="https://collaboration.mdlz.com/:b:/r/sites/alteryx/Shared Documents/Alteryx Incident Creation in Service Now (SNOW).pdf?csf=1&amp;web=1&amp;e=TCJuLt" xr:uid="{532682CB-D8D4-4722-A56E-FAEE2E8385E9}"/>
-    <hyperlink ref="E135" r:id="rId247" display="https://collaboration.mdlz.com/:b:/r/sites/alteryx/Shared Documents/Alteryx Training/Alteryx Inhouse Training by Vendor.pdf?csf=1&amp;web=1&amp;e=JrCtym" xr:uid="{AD3A5E16-2403-4C83-8CF2-4DA62BA44B5C}"/>
-    <hyperlink ref="E136" r:id="rId248" xr:uid="{E7BAA7FD-6AA1-4FDF-8F9B-F90BE340B991}"/>
-    <hyperlink ref="E137" r:id="rId249" display="https://collaboration.mdlz.com/:f:/r/sites/AecorSoft/Shared Documents/Developer Guides?csf=1&amp;web=1&amp;e=ibnmci" xr:uid="{BE62D4E0-45AA-429E-B891-0BBC6F72DE74}"/>
-    <hyperlink ref="E138" r:id="rId250" display="https://collaboration.mdlz.com/:b:/r/sites/AecorSoft/Shared Documents/Aecrosoft_Incident_Creation_SNOW.pdf?csf=1&amp;web=1&amp;e=PhhiaJ" xr:uid="{EB53023E-5521-468F-AD4A-FB9B65365CEC}"/>
-    <hyperlink ref="E141" r:id="rId251" location="sap-bi-platform" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Service-catalogue.aspx - sap-bi-platform" xr:uid="{4555F72F-2E17-4E72-9737-FAA89420B6F1}"/>
-    <hyperlink ref="E144" r:id="rId252" xr:uid="{394E101A-FB32-4FFC-B52C-498202901E5C}"/>
-    <hyperlink ref="E147" r:id="rId253" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Pre Prod Readiness.aspx?csf=1&amp;web=1&amp;e=kbE51k" xr:uid="{C0E0FD79-11FF-4E48-8591-06EEA45901F8}"/>
-    <hyperlink ref="E148" r:id="rId254" location="expectation-from-product-teams" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Pre Prod Readiness.aspx?csf=1&amp;web=1&amp;e=kbE51k - expectation-from-product-teams" xr:uid="{8EBF64D3-4E70-467E-8E73-0561431C269B}"/>
+    <hyperlink ref="E129" r:id="rId243" location="data-integration-platforms" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Service-catalogue.aspx - data-integration-platforms" xr:uid="{DBCD28CC-93A8-4C9B-B4E9-44A5D42822E4}"/>
+    <hyperlink ref="E130" r:id="rId244" display="https://collaboration.mdlz.com/:b:/r/sites/alteryx/Shared Documents/Guidlines for Alteryx usage- MDLZ.pdf?csf=1&amp;web=1&amp;e=owyGdK" xr:uid="{13C082D6-C3B9-4755-A934-E699194D8CDE}"/>
+    <hyperlink ref="E131" r:id="rId245" display="https://collaboration.mdlz.com/:b:/r/sites/alteryx/Shared Documents/Alteryx New Project Setup %26 Best Practices.pdf?csf=1&amp;web=1&amp;e=2NAIcG" xr:uid="{4F8EA5C5-572E-45D0-8906-E57D0525F255}"/>
+    <hyperlink ref="E132" r:id="rId246" display="https://collaboration.mdlz.com/:b:/r/sites/alteryx/Shared Documents/Alteryx Incident Creation in Service Now (SNOW).pdf?csf=1&amp;web=1&amp;e=TCJuLt" xr:uid="{532682CB-D8D4-4722-A56E-FAEE2E8385E9}"/>
+    <hyperlink ref="E133" r:id="rId247" display="https://collaboration.mdlz.com/:b:/r/sites/alteryx/Shared Documents/Alteryx Training/Alteryx Inhouse Training by Vendor.pdf?csf=1&amp;web=1&amp;e=JrCtym" xr:uid="{AD3A5E16-2403-4C83-8CF2-4DA62BA44B5C}"/>
+    <hyperlink ref="E134" r:id="rId248" xr:uid="{E7BAA7FD-6AA1-4FDF-8F9B-F90BE340B991}"/>
+    <hyperlink ref="E135" r:id="rId249" display="https://collaboration.mdlz.com/:f:/r/sites/AecorSoft/Shared Documents/Developer Guides?csf=1&amp;web=1&amp;e=ibnmci" xr:uid="{BE62D4E0-45AA-429E-B891-0BBC6F72DE74}"/>
+    <hyperlink ref="E136" r:id="rId250" display="https://collaboration.mdlz.com/:b:/r/sites/AecorSoft/Shared Documents/Aecrosoft_Incident_Creation_SNOW.pdf?csf=1&amp;web=1&amp;e=PhhiaJ" xr:uid="{EB53023E-5521-468F-AD4A-FB9B65365CEC}"/>
+    <hyperlink ref="E137" r:id="rId251" location="sap-bi-platform" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Service-catalogue.aspx - sap-bi-platform" xr:uid="{4555F72F-2E17-4E72-9737-FAA89420B6F1}"/>
+    <hyperlink ref="E138" r:id="rId252" xr:uid="{394E101A-FB32-4FFC-B52C-498202901E5C}"/>
+    <hyperlink ref="E139" r:id="rId253" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Pre Prod Readiness.aspx?csf=1&amp;web=1&amp;e=kbE51k" xr:uid="{C0E0FD79-11FF-4E48-8591-06EEA45901F8}"/>
+    <hyperlink ref="E140" r:id="rId254" location="expectation-from-product-teams" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Pre Prod Readiness.aspx?csf=1&amp;web=1&amp;e=kbE51k - expectation-from-product-teams" xr:uid="{8EBF64D3-4E70-467E-8E73-0561431C269B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId255"/>

</xml_diff>

<commit_message>
Added questions for data science
</commit_message>
<xml_diff>
--- a/data/chatbot-1.xlsx
+++ b/data/chatbot-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJK3794\PycharmProjects\Datahub Chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5AAF31-3EA6-44E3-8F5A-6B63211D08FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7183B6-895A-4B57-9FAC-800E487E2B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{CB1DE796-0A7F-4358-B0F5-62D7433C0693}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="545">
   <si>
     <t>Category</t>
   </si>
@@ -1242,6 +1242,441 @@
   </si>
   <si>
     <t>Pre-Prod Expectations from Product Team</t>
+  </si>
+  <si>
+    <t>Data Science COE</t>
+  </si>
+  <si>
+    <t>Getting started</t>
+  </si>
+  <si>
+    <t>What is MLOps</t>
+  </si>
+  <si>
+    <t>Why is  MLOps needed?</t>
+  </si>
+  <si>
+    <t>What are the different components in MLOps</t>
+  </si>
+  <si>
+    <t>What is the folder structure of MLOps enabled Data Science project</t>
+  </si>
+  <si>
+    <t>Machine Learning Lifecycle</t>
+  </si>
+  <si>
+    <t>What is the standard ML lifecycle in Mdlz?</t>
+  </si>
+  <si>
+    <t>How to perform MVP assessment of a data science application?</t>
+  </si>
+  <si>
+    <t>How to perform pre-industrialization assessment of a data science application?</t>
+  </si>
+  <si>
+    <t>Is my application ready for impelmenting MLOPs?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How should minor enhancements for data science applications be handled? </t>
+  </si>
+  <si>
+    <t>How should major enhancements for data science applications be handled?</t>
+  </si>
+  <si>
+    <t>Development guidelines</t>
+  </si>
+  <si>
+    <t>What guidelines should be followed when developing Data Science applications?</t>
+  </si>
+  <si>
+    <t>What is MLOps compliance checklist?</t>
+  </si>
+  <si>
+    <t>What coding practices should be followed during the devlopment of Data Science applications?</t>
+  </si>
+  <si>
+    <t>MLOPS components</t>
+  </si>
+  <si>
+    <t>How do I get started with MLOps in my git repository?</t>
+  </si>
+  <si>
+    <t>What are data quality checks?</t>
+  </si>
+  <si>
+    <t>What is data validation?</t>
+  </si>
+  <si>
+    <t>What are the benefits of data validation?</t>
+  </si>
+  <si>
+    <t>How can I setup data validation using MLOps?</t>
+  </si>
+  <si>
+    <t>What is a feature store?</t>
+  </si>
+  <si>
+    <t>what are the benefits of enabling feature store?</t>
+  </si>
+  <si>
+    <t>Give an example of feature store implementation</t>
+  </si>
+  <si>
+    <t>What is data drift?</t>
+  </si>
+  <si>
+    <t>How is data drift detected?</t>
+  </si>
+  <si>
+    <t>Give an example of data drift detection implementation?</t>
+  </si>
+  <si>
+    <t>What is experiment tracking?</t>
+  </si>
+  <si>
+    <t>How to manage versions of machine learning models?</t>
+  </si>
+  <si>
+    <t>How to make modelling process more transparent?</t>
+  </si>
+  <si>
+    <t>How to track model performance efficiently?</t>
+  </si>
+  <si>
+    <t>How do I stay updated on my Machine Learning projects?</t>
+  </si>
+  <si>
+    <t>Where are the Machine Learning models stored?</t>
+  </si>
+  <si>
+    <t>How can I roll back to the previous model version?</t>
+  </si>
+  <si>
+    <t>What is modelOps process?</t>
+  </si>
+  <si>
+    <t>What is model registry?</t>
+  </si>
+  <si>
+    <t>What is model drift?</t>
+  </si>
+  <si>
+    <t>Why is model drift detection needed?</t>
+  </si>
+  <si>
+    <t>what tools are used to detect model drift?</t>
+  </si>
+  <si>
+    <t>Give an example of model drift implementation?</t>
+  </si>
+  <si>
+    <t>How are Machine learning models deployed?</t>
+  </si>
+  <si>
+    <t>What is model serving?</t>
+  </si>
+  <si>
+    <t>How to deploy machine learning models in production?</t>
+  </si>
+  <si>
+    <t>What is model explainability?</t>
+  </si>
+  <si>
+    <t>How can I interpret my model's predictions?</t>
+  </si>
+  <si>
+    <t>What tools are used for model explainability?</t>
+  </si>
+  <si>
+    <t>DevOps for data science</t>
+  </si>
+  <si>
+    <t>How do I roll back my entire ML application?</t>
+  </si>
+  <si>
+    <t>How can I implement CI/CD for my data science application?</t>
+  </si>
+  <si>
+    <t>What is the git branching strategy in MLOps enabled projects?</t>
+  </si>
+  <si>
+    <t>What is CI/CD?</t>
+  </si>
+  <si>
+    <t>What is Continuous integration of code?</t>
+  </si>
+  <si>
+    <t>What is COntinuous deployment of code?</t>
+  </si>
+  <si>
+    <t>What is the approval process for codes?</t>
+  </si>
+  <si>
+    <t>How to enable sonarqube in mdlz?</t>
+  </si>
+  <si>
+    <t>How can sonarqube help my application?</t>
+  </si>
+  <si>
+    <t>What insights can I get from sonarqube?</t>
+  </si>
+  <si>
+    <t>How can I assess the technical debt in my application?</t>
+  </si>
+  <si>
+    <t>How to parameterize my data science application?</t>
+  </si>
+  <si>
+    <t>How to deploy databricks workflows in higher environments?</t>
+  </si>
+  <si>
+    <t>How do I move my code to production?</t>
+  </si>
+  <si>
+    <t>How do I pass credentials to my data science application in databricks?</t>
+  </si>
+  <si>
+    <t>How do I pass confidential parameters to my data science applications?</t>
+  </si>
+  <si>
+    <t>How is logging managed as a part of MLOps?</t>
+  </si>
+  <si>
+    <t>Monitoring &amp; Logging</t>
+  </si>
+  <si>
+    <t>Where are the MLOps monitoring logs stored?</t>
+  </si>
+  <si>
+    <t>What is Information Lifecycle Management?</t>
+  </si>
+  <si>
+    <t>How is historical data managed in MLOps?</t>
+  </si>
+  <si>
+    <t>How do I monitor my resource utilization in databricks?</t>
+  </si>
+  <si>
+    <t>How can spark code be optimized?</t>
+  </si>
+  <si>
+    <t>MLOPs educational sessions</t>
+  </si>
+  <si>
+    <t>Where can I find more information on MLOPs?</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/MLOps_Getting_Started_Document.html#what-is-mlops</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/MLOps_Getting_Started_Document.html#what-are-the-key-challenges-we-intend-to-solve-with-mlops</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/MLOps_Getting_Started_Document.html#mlops-components</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/MLOps_Getting_Started_Document.html#how-to-access-rep</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Machine-Learning-Life-Cycle.html#ml-life-cycle</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Machine-Learning-Life-Cycle.html#mvp-assessment</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Machine-Learning-Life-Cycle.html#pre-industrialization-assessment</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Minor-Enhancement-Workflow.html#minor-enhancement-workflow</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Major-Enhancement-workflow.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Compliance_Checklist.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/SettingUp-MLOps-Workflow.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Data-Validation.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Data-Validation.html#introduction-to-data-validation--its-benefits</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Feature-Store.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Feature-Store.html#introduction-to-feature-stores--its-benefits</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Data-Drift.html#introduction-to-data-drift-and-its-benefits</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Data-Drift.html#tools-for-detecting-data-drift</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Data-Drift.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Model-Experiments.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/SettingUp-Model-Registry-Webhook.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Model-Registry.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Model_Approval_Process.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Model-Drift.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Model-Drift.html#introduction-to-model-drift-and-its-benefits</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Model-Drift.html#tools-for-detecting-model-drift</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Model-Serving.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Model-Explainability.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Model-Explainability.html#frameworks-for-model-xai</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/cicd-strategy.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/cicd-strategy.html#7-continuous-integration-ci</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/cicd-strategy.html#8-continuous-delivery</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/ace-market-place/docs/url=https%3A%2F%2Finsight.mdlz.com%2Fp%2Fd4gvdocs%2FDSGovernance%2Fcicd-strategy.html%2310-github-pull-request-approval-gateway</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/sonarqube_integration.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/sonarqube-analysis-report.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/sonarqube-analysis-report.html#debt</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/cd-pre-requisites.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/cd-job-definition-guide.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Databricks-Secret-Scope.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Generic-Log-Management.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Information-Lifecycle-Management.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Workflow-Performance-Monitoring.html#workflow-performance-montoring</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Pyspark_Guide.html</t>
+  </si>
+  <si>
+    <t>https://insight.mdlz.com/p/d4gvdocs/DSGovernance/Educational-Sessions.html</t>
+  </si>
+  <si>
+    <t>MLOps Getting Started</t>
+  </si>
+  <si>
+    <t>Machine Learning Life Cycle</t>
+  </si>
+  <si>
+    <t>Minor Enhancement Workflow</t>
+  </si>
+  <si>
+    <t>Major Enhancement workflow</t>
+  </si>
+  <si>
+    <t>Compliance Checklist</t>
+  </si>
+  <si>
+    <t>Data Validation</t>
+  </si>
+  <si>
+    <t>Feature Store</t>
+  </si>
+  <si>
+    <t>Data Drift</t>
+  </si>
+  <si>
+    <t>Model Experiments</t>
+  </si>
+  <si>
+    <t>Model Registry</t>
+  </si>
+  <si>
+    <t>Model Drift</t>
+  </si>
+  <si>
+    <t>Model Serving</t>
+  </si>
+  <si>
+    <t>Model Explainability</t>
+  </si>
+  <si>
+    <t>Setting Up MLOps Workflow</t>
+  </si>
+  <si>
+    <t>SettingUp Model-Registry-Webhook</t>
+  </si>
+  <si>
+    <t>Pyspark Guide</t>
+  </si>
+  <si>
+    <t>Educational Sessions</t>
+  </si>
+  <si>
+    <t>CI/CD Strategy</t>
+  </si>
+  <si>
+    <t>Model_Approval Experiments</t>
+  </si>
+  <si>
+    <t>CI/L= Market-Place/Docs/Url=Https%3A%2F%2Finsight.Mdlz.Com%2Fp%2Fd4Gvdocs%2Fdsgovernance%2Fcicd-Strategy</t>
+  </si>
+  <si>
+    <t>CI/NARQUBE_INTEGRATION.HTML Integration</t>
+  </si>
+  <si>
+    <t>CI/NARQUBE Analysis-Report</t>
+  </si>
+  <si>
+    <t>Workflow Performance Monitoring</t>
+  </si>
+  <si>
+    <t>Information Lifecycle Management</t>
+  </si>
+  <si>
+    <t>CD Pre-Requisites</t>
+  </si>
+  <si>
+    <t>CD Job-Definition-Guide</t>
+  </si>
+  <si>
+    <t>DATABRICKS Secret-Scope</t>
+  </si>
+  <si>
+    <t>GENERIC Log-Management</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1368,6 +1803,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1685,11 +2125,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}">
-  <dimension ref="A1:L140"/>
+  <dimension ref="A1:L206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="87" zoomScaleNormal="72" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B129" activeCellId="1" sqref="A134:XFD134 A129:XFD129"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A142" sqref="A142:A206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1698,7 +2138,7 @@
     <col min="2" max="2" width="43.26953125" customWidth="1"/>
     <col min="3" max="3" width="40.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.54296875" customWidth="1"/>
+    <col min="5" max="5" width="105.7265625" customWidth="1"/>
     <col min="6" max="6" width="106" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.90625" bestFit="1" customWidth="1"/>
@@ -4611,6 +5051,1326 @@
       </c>
       <c r="F140" t="s">
         <v>399</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>400</v>
+      </c>
+      <c r="B141" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="C141" t="s">
+        <v>401</v>
+      </c>
+      <c r="D141" t="s">
+        <v>402</v>
+      </c>
+      <c r="E141" s="18" t="s">
+        <v>474</v>
+      </c>
+      <c r="F141" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B142" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="C142" t="s">
+        <v>401</v>
+      </c>
+      <c r="D142" t="s">
+        <v>403</v>
+      </c>
+      <c r="E142" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="F142" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B143" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="C143" t="s">
+        <v>401</v>
+      </c>
+      <c r="D143" t="s">
+        <v>404</v>
+      </c>
+      <c r="E143" s="18" t="s">
+        <v>476</v>
+      </c>
+      <c r="F143" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B144" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="C144" t="s">
+        <v>401</v>
+      </c>
+      <c r="D144" t="s">
+        <v>405</v>
+      </c>
+      <c r="E144" s="18" t="s">
+        <v>477</v>
+      </c>
+      <c r="F144" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A145" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B145" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C145" t="s">
+        <v>406</v>
+      </c>
+      <c r="D145" t="s">
+        <v>407</v>
+      </c>
+      <c r="E145" s="18" t="s">
+        <v>478</v>
+      </c>
+      <c r="F145" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A146" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B146" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C146" t="s">
+        <v>406</v>
+      </c>
+      <c r="D146" t="s">
+        <v>408</v>
+      </c>
+      <c r="E146" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="F146" s="17" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A147" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C147" t="s">
+        <v>406</v>
+      </c>
+      <c r="D147" t="s">
+        <v>409</v>
+      </c>
+      <c r="E147" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="F147" s="17" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A148" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B148" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C148" t="s">
+        <v>406</v>
+      </c>
+      <c r="D148" t="s">
+        <v>410</v>
+      </c>
+      <c r="E148" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="F148" s="17" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A149" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B149" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C149" t="s">
+        <v>406</v>
+      </c>
+      <c r="D149" t="s">
+        <v>411</v>
+      </c>
+      <c r="E149" s="18" t="s">
+        <v>481</v>
+      </c>
+      <c r="F149" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A150" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B150" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C150" t="s">
+        <v>406</v>
+      </c>
+      <c r="D150" t="s">
+        <v>412</v>
+      </c>
+      <c r="E150" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="F150" s="17" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A151" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B151" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="C151" t="s">
+        <v>413</v>
+      </c>
+      <c r="D151" t="s">
+        <v>414</v>
+      </c>
+      <c r="E151" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="F151" s="17" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A152" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B152" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="C152" t="s">
+        <v>413</v>
+      </c>
+      <c r="D152" t="s">
+        <v>415</v>
+      </c>
+      <c r="E152" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="F152" s="17" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A153" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B153" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="C153" t="s">
+        <v>413</v>
+      </c>
+      <c r="D153" t="s">
+        <v>416</v>
+      </c>
+      <c r="E153" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="F153" s="17" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A154" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B154" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C154" t="s">
+        <v>417</v>
+      </c>
+      <c r="D154" t="s">
+        <v>418</v>
+      </c>
+      <c r="E154" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="F154" s="17" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A155" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B155" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C155" t="s">
+        <v>417</v>
+      </c>
+      <c r="D155" t="s">
+        <v>419</v>
+      </c>
+      <c r="E155" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="F155" s="17" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A156" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B156" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C156" t="s">
+        <v>417</v>
+      </c>
+      <c r="D156" t="s">
+        <v>420</v>
+      </c>
+      <c r="E156" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="F156" s="17" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A157" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B157" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C157" t="s">
+        <v>417</v>
+      </c>
+      <c r="D157" t="s">
+        <v>421</v>
+      </c>
+      <c r="E157" s="18" t="s">
+        <v>486</v>
+      </c>
+      <c r="F157" s="17" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A158" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B158" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C158" t="s">
+        <v>417</v>
+      </c>
+      <c r="D158" t="s">
+        <v>422</v>
+      </c>
+      <c r="E158" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="F158" s="17" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A159" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B159" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C159" t="s">
+        <v>417</v>
+      </c>
+      <c r="D159" t="s">
+        <v>423</v>
+      </c>
+      <c r="E159" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="F159" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A160" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B160" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C160" t="s">
+        <v>417</v>
+      </c>
+      <c r="D160" t="s">
+        <v>424</v>
+      </c>
+      <c r="E160" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="F160" s="17" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A161" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B161" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C161" t="s">
+        <v>417</v>
+      </c>
+      <c r="D161" t="s">
+        <v>425</v>
+      </c>
+      <c r="E161" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="F161" s="17" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A162" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B162" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C162" t="s">
+        <v>417</v>
+      </c>
+      <c r="D162" t="s">
+        <v>426</v>
+      </c>
+      <c r="E162" s="18" t="s">
+        <v>489</v>
+      </c>
+      <c r="F162" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A163" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B163" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C163" t="s">
+        <v>417</v>
+      </c>
+      <c r="D163" t="s">
+        <v>427</v>
+      </c>
+      <c r="E163" s="18" t="s">
+        <v>490</v>
+      </c>
+      <c r="F163" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A164" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B164" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C164" t="s">
+        <v>417</v>
+      </c>
+      <c r="D164" t="s">
+        <v>428</v>
+      </c>
+      <c r="E164" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="F164" s="17" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A165" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B165" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C165" t="s">
+        <v>417</v>
+      </c>
+      <c r="D165" t="s">
+        <v>429</v>
+      </c>
+      <c r="E165" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="F165" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A166" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B166" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C166" t="s">
+        <v>417</v>
+      </c>
+      <c r="D166" t="s">
+        <v>430</v>
+      </c>
+      <c r="E166" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="F166" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A167" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B167" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C167" t="s">
+        <v>417</v>
+      </c>
+      <c r="D167" t="s">
+        <v>431</v>
+      </c>
+      <c r="E167" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="F167" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A168" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B168" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C168" t="s">
+        <v>417</v>
+      </c>
+      <c r="D168" t="s">
+        <v>432</v>
+      </c>
+      <c r="E168" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="F168" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A169" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B169" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C169" t="s">
+        <v>417</v>
+      </c>
+      <c r="D169" t="s">
+        <v>433</v>
+      </c>
+      <c r="E169" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="F169" s="17" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A170" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B170" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C170" t="s">
+        <v>417</v>
+      </c>
+      <c r="D170" t="s">
+        <v>434</v>
+      </c>
+      <c r="E170" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="F170" s="17" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A171" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B171" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C171" t="s">
+        <v>417</v>
+      </c>
+      <c r="D171" t="s">
+        <v>435</v>
+      </c>
+      <c r="E171" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="F171" s="17" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A172" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B172" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C172" t="s">
+        <v>417</v>
+      </c>
+      <c r="D172" t="s">
+        <v>436</v>
+      </c>
+      <c r="E172" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="F172" s="17" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A173" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B173" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C173" t="s">
+        <v>417</v>
+      </c>
+      <c r="D173" t="s">
+        <v>437</v>
+      </c>
+      <c r="E173" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="F173" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A174" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B174" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C174" t="s">
+        <v>417</v>
+      </c>
+      <c r="D174" t="s">
+        <v>438</v>
+      </c>
+      <c r="E174" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="F174" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A175" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B175" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C175" t="s">
+        <v>417</v>
+      </c>
+      <c r="D175" t="s">
+        <v>439</v>
+      </c>
+      <c r="E175" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="F175" s="17" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A176" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B176" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C176" t="s">
+        <v>417</v>
+      </c>
+      <c r="D176" t="s">
+        <v>440</v>
+      </c>
+      <c r="E176" s="18" t="s">
+        <v>498</v>
+      </c>
+      <c r="F176" s="17" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A177" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B177" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C177" t="s">
+        <v>417</v>
+      </c>
+      <c r="D177" t="s">
+        <v>441</v>
+      </c>
+      <c r="E177" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="F177" s="17" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A178" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B178" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C178" t="s">
+        <v>417</v>
+      </c>
+      <c r="D178" t="s">
+        <v>442</v>
+      </c>
+      <c r="E178" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="F178" s="17" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A179" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B179" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C179" t="s">
+        <v>417</v>
+      </c>
+      <c r="D179" t="s">
+        <v>443</v>
+      </c>
+      <c r="E179" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="F179" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A180" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B180" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C180" t="s">
+        <v>417</v>
+      </c>
+      <c r="D180" t="s">
+        <v>444</v>
+      </c>
+      <c r="E180" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="F180" s="17" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A181" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B181" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C181" t="s">
+        <v>417</v>
+      </c>
+      <c r="D181" t="s">
+        <v>445</v>
+      </c>
+      <c r="E181" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="F181" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A182" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B182" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C182" t="s">
+        <v>417</v>
+      </c>
+      <c r="D182" t="s">
+        <v>446</v>
+      </c>
+      <c r="E182" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="F182" s="17" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A183" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B183" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C183" t="s">
+        <v>417</v>
+      </c>
+      <c r="D183" t="s">
+        <v>447</v>
+      </c>
+      <c r="E183" s="18" t="s">
+        <v>501</v>
+      </c>
+      <c r="F183" s="17" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A184" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B184" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C184" t="s">
+        <v>448</v>
+      </c>
+      <c r="D184" t="s">
+        <v>449</v>
+      </c>
+      <c r="E184" s="18" t="s">
+        <v>502</v>
+      </c>
+      <c r="F184" s="17" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A185" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B185" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C185" t="s">
+        <v>448</v>
+      </c>
+      <c r="D185" t="s">
+        <v>450</v>
+      </c>
+      <c r="E185" s="18" t="s">
+        <v>502</v>
+      </c>
+      <c r="F185" s="17" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A186" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B186" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C186" t="s">
+        <v>448</v>
+      </c>
+      <c r="D186" t="s">
+        <v>451</v>
+      </c>
+      <c r="E186" s="18" t="s">
+        <v>502</v>
+      </c>
+      <c r="F186" s="17" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A187" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B187" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C187" t="s">
+        <v>448</v>
+      </c>
+      <c r="D187" t="s">
+        <v>452</v>
+      </c>
+      <c r="E187" s="18" t="s">
+        <v>502</v>
+      </c>
+      <c r="F187" s="17" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A188" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B188" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C188" t="s">
+        <v>448</v>
+      </c>
+      <c r="D188" t="s">
+        <v>453</v>
+      </c>
+      <c r="E188" s="18" t="s">
+        <v>503</v>
+      </c>
+      <c r="F188" s="17" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A189" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B189" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C189" t="s">
+        <v>448</v>
+      </c>
+      <c r="D189" t="s">
+        <v>454</v>
+      </c>
+      <c r="E189" s="18" t="s">
+        <v>504</v>
+      </c>
+      <c r="F189" s="17" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A190" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B190" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C190" t="s">
+        <v>448</v>
+      </c>
+      <c r="D190" t="s">
+        <v>455</v>
+      </c>
+      <c r="E190" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="F190" s="17" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A191" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B191" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C191" t="s">
+        <v>448</v>
+      </c>
+      <c r="D191" t="s">
+        <v>456</v>
+      </c>
+      <c r="E191" s="18" t="s">
+        <v>506</v>
+      </c>
+      <c r="F191" s="17" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A192" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B192" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C192" t="s">
+        <v>448</v>
+      </c>
+      <c r="D192" t="s">
+        <v>457</v>
+      </c>
+      <c r="E192" s="18" t="s">
+        <v>507</v>
+      </c>
+      <c r="F192" s="17" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A193" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B193" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C193" t="s">
+        <v>448</v>
+      </c>
+      <c r="D193" t="s">
+        <v>458</v>
+      </c>
+      <c r="E193" s="18" t="s">
+        <v>507</v>
+      </c>
+      <c r="F193" s="17" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A194" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B194" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C194" t="s">
+        <v>448</v>
+      </c>
+      <c r="D194" t="s">
+        <v>459</v>
+      </c>
+      <c r="E194" s="18" t="s">
+        <v>508</v>
+      </c>
+      <c r="F194" s="17" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A195" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B195" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C195" t="s">
+        <v>448</v>
+      </c>
+      <c r="D195" t="s">
+        <v>460</v>
+      </c>
+      <c r="E195" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="F195" s="17" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B196" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C196" t="s">
+        <v>448</v>
+      </c>
+      <c r="D196" t="s">
+        <v>461</v>
+      </c>
+      <c r="E196" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="F196" s="17" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A197" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B197" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C197" t="s">
+        <v>448</v>
+      </c>
+      <c r="D197" t="s">
+        <v>462</v>
+      </c>
+      <c r="E197" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="F197" s="17" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A198" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B198" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C198" t="s">
+        <v>448</v>
+      </c>
+      <c r="D198" t="s">
+        <v>463</v>
+      </c>
+      <c r="E198" s="18" t="s">
+        <v>511</v>
+      </c>
+      <c r="F198" s="17" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A199" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B199" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C199" t="s">
+        <v>448</v>
+      </c>
+      <c r="D199" t="s">
+        <v>464</v>
+      </c>
+      <c r="E199" s="18" t="s">
+        <v>511</v>
+      </c>
+      <c r="F199" s="17" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A200" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B200" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="C200" t="s">
+        <v>448</v>
+      </c>
+      <c r="D200" t="s">
+        <v>465</v>
+      </c>
+      <c r="E200" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="F200" s="17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A201" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B201" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="C201" t="s">
+        <v>466</v>
+      </c>
+      <c r="D201" t="s">
+        <v>467</v>
+      </c>
+      <c r="E201" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="F201" s="17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A202" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B202" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="C202" t="s">
+        <v>466</v>
+      </c>
+      <c r="D202" t="s">
+        <v>468</v>
+      </c>
+      <c r="E202" s="18" t="s">
+        <v>513</v>
+      </c>
+      <c r="F202" s="17" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A203" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B203" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="C203" t="s">
+        <v>466</v>
+      </c>
+      <c r="D203" t="s">
+        <v>469</v>
+      </c>
+      <c r="E203" s="18" t="s">
+        <v>513</v>
+      </c>
+      <c r="F203" s="17" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A204" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B204" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="C204" t="s">
+        <v>466</v>
+      </c>
+      <c r="D204" t="s">
+        <v>470</v>
+      </c>
+      <c r="E204" s="18" t="s">
+        <v>514</v>
+      </c>
+      <c r="F204" s="17" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A205" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B205" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="C205" t="s">
+        <v>413</v>
+      </c>
+      <c r="D205" t="s">
+        <v>471</v>
+      </c>
+      <c r="E205" s="18" t="s">
+        <v>515</v>
+      </c>
+      <c r="F205" s="17" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A206" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B206" s="17" t="s">
+        <v>472</v>
+      </c>
+      <c r="C206" t="s">
+        <v>472</v>
+      </c>
+      <c r="D206" t="s">
+        <v>473</v>
+      </c>
+      <c r="E206" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="F206" s="17" t="s">
+        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -4870,9 +6630,80 @@
     <hyperlink ref="E138" r:id="rId252" xr:uid="{394E101A-FB32-4FFC-B52C-498202901E5C}"/>
     <hyperlink ref="E139" r:id="rId253" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Pre Prod Readiness.aspx?csf=1&amp;web=1&amp;e=kbE51k" xr:uid="{C0E0FD79-11FF-4E48-8591-06EEA45901F8}"/>
     <hyperlink ref="E140" r:id="rId254" location="expectation-from-product-teams" display="https://collaboration.mdlz.com/sites/MDSDataAnalyticsPlatforms/SitePages/Pre Prod Readiness.aspx?csf=1&amp;web=1&amp;e=kbE51k - expectation-from-product-teams" xr:uid="{8EBF64D3-4E70-467E-8E73-0561431C269B}"/>
+    <hyperlink ref="E141" r:id="rId255" location="what-is-mlops" xr:uid="{C8976EDF-B239-45E0-A758-4D8DF246940C}"/>
+    <hyperlink ref="E142" r:id="rId256" location="what-are-the-key-challenges-we-intend-to-solve-with-mlops" xr:uid="{46B921A2-5BA1-4F34-B34E-B7A057F57912}"/>
+    <hyperlink ref="E153:E172" r:id="rId257" display="https://insight.mdlz.com/p/" xr:uid="{5C7B1B90-78E4-45B9-AE89-7FED373B06B3}"/>
+    <hyperlink ref="E143:E154" r:id="rId258" display="https://insight.mdlz.com/p/d4gvdocs" xr:uid="{27E25457-87E2-41B2-909C-A2BC0CD41602}"/>
+    <hyperlink ref="E155:E179" r:id="rId259" display="https://insight.mdlz.com/p/" xr:uid="{27B40690-2D5B-403C-AEEA-749F8DB69EF9}"/>
+    <hyperlink ref="E190" r:id="rId260" xr:uid="{64455EDB-2139-43D4-8205-61EF55408519}"/>
+    <hyperlink ref="E143" r:id="rId261" location="mlops-components" xr:uid="{F52AFB75-C423-4D37-BBF4-46CF9B39C536}"/>
+    <hyperlink ref="E144" r:id="rId262" location="how-to-access-rep" xr:uid="{C85870FF-556B-4C73-A616-AAFAA63390FF}"/>
+    <hyperlink ref="E145" r:id="rId263" location="ml-life-cycle" xr:uid="{725B8B13-A1D9-47B5-85BD-FD20E7D80EB2}"/>
+    <hyperlink ref="E146" r:id="rId264" location="mvp-assessment" xr:uid="{CAE8FF48-B44B-43B8-BCC8-5DD35411BFA6}"/>
+    <hyperlink ref="E147" r:id="rId265" location="pre-industrialization-assessment" xr:uid="{92406200-6890-4180-AD34-08E6DC0424ED}"/>
+    <hyperlink ref="E148" r:id="rId266" location="pre-industrialization-assessment" xr:uid="{00507435-5CFC-4C4C-B326-2921CF0AC720}"/>
+    <hyperlink ref="E149" r:id="rId267" location="minor-enhancement-workflow" xr:uid="{DA9F75C0-911C-40B6-B3E9-D131EC615B50}"/>
+    <hyperlink ref="E150" r:id="rId268" xr:uid="{1B87E866-C103-49FD-B70D-1BB3F807402A}"/>
+    <hyperlink ref="E151" r:id="rId269" xr:uid="{75C0A138-F66B-4485-9428-B898043775BE}"/>
+    <hyperlink ref="E152" r:id="rId270" xr:uid="{D6EA4E02-2E89-4352-8BF9-204C2D289436}"/>
+    <hyperlink ref="E153" r:id="rId271" xr:uid="{AA954110-E720-400D-9945-83660136C5B8}"/>
+    <hyperlink ref="E154" r:id="rId272" xr:uid="{9B2E995B-8FDE-4D11-B29B-B698BA78E15F}"/>
+    <hyperlink ref="E155" r:id="rId273" xr:uid="{AF4824DF-1F2C-47E6-8EF1-4E4D7F0E7BB1}"/>
+    <hyperlink ref="E156" r:id="rId274" xr:uid="{7F08D811-70B2-436A-8AFB-CA8A4AD86AC7}"/>
+    <hyperlink ref="E157" r:id="rId275" location="introduction-to-data-validation--its-benefits" xr:uid="{62A20442-5717-409A-B105-DCF57E1B5314}"/>
+    <hyperlink ref="E158" r:id="rId276" xr:uid="{7C58051B-505A-4C87-B85B-4A434BCFF1B5}"/>
+    <hyperlink ref="E159" r:id="rId277" xr:uid="{FE5CE63F-7607-4116-BAB4-FCBDCFF402C7}"/>
+    <hyperlink ref="E160" r:id="rId278" location="introduction-to-feature-stores--its-benefits" xr:uid="{D15F0168-E6C5-4C5B-8EBE-05324283B7D4}"/>
+    <hyperlink ref="E161" r:id="rId279" xr:uid="{C6613939-BB2E-4ED5-9BE2-BB5DC3AE9294}"/>
+    <hyperlink ref="E162" r:id="rId280" location="introduction-to-data-drift-and-its-benefits" xr:uid="{CBA77768-CC2C-4457-92C7-4073A28292BF}"/>
+    <hyperlink ref="E163" r:id="rId281" location="tools-for-detecting-data-drift" xr:uid="{2C81750D-1352-4012-9CE5-07E47EC3DE3F}"/>
+    <hyperlink ref="E164" r:id="rId282" xr:uid="{2EC3D27E-025D-40D2-B7E7-AF3E64D547F8}"/>
+    <hyperlink ref="E165" r:id="rId283" xr:uid="{FCC8D865-E9FE-4985-AAB7-ECBF4D196ED9}"/>
+    <hyperlink ref="E166" r:id="rId284" xr:uid="{FD675F2F-F4C7-4CD8-82E8-583798C35ABD}"/>
+    <hyperlink ref="E167" r:id="rId285" xr:uid="{09D649B1-0EAC-427F-946B-1B92BF94B36D}"/>
+    <hyperlink ref="E168" r:id="rId286" xr:uid="{A6B96C2A-6408-435C-9D9C-EF227813D60C}"/>
+    <hyperlink ref="E169" r:id="rId287" xr:uid="{E98E07E4-B96F-4FC9-BCC2-DAA3469362AE}"/>
+    <hyperlink ref="E170" r:id="rId288" xr:uid="{1A2668A1-C674-4475-97EC-E8DD9243EEB4}"/>
+    <hyperlink ref="E171" r:id="rId289" xr:uid="{0015D9B9-45D8-45BA-AC45-0BB4AFD88C07}"/>
+    <hyperlink ref="E172" r:id="rId290" xr:uid="{7EE3727A-D81A-4FA5-AB2F-361FEEB32315}"/>
+    <hyperlink ref="E173" r:id="rId291" xr:uid="{172907A3-CE9E-41B2-B9DE-EDF605F02737}"/>
+    <hyperlink ref="E174" r:id="rId292" xr:uid="{0A3B9156-D66B-4EB3-9E54-C3305A93D96A}"/>
+    <hyperlink ref="E175" r:id="rId293" location="introduction-to-model-drift-and-its-benefits" xr:uid="{B11F5A27-9846-4CCE-BB35-623DD7461645}"/>
+    <hyperlink ref="E176" r:id="rId294" location="tools-for-detecting-model-drift" xr:uid="{2656C42B-CF2E-48F6-A991-D2700ED8C6E2}"/>
+    <hyperlink ref="E177" r:id="rId295" xr:uid="{A97DD643-83D5-4B21-9181-3C6147F53368}"/>
+    <hyperlink ref="E178" r:id="rId296" xr:uid="{C9605C89-18CC-4E09-8CB4-70A97E73AE41}"/>
+    <hyperlink ref="E179" r:id="rId297" xr:uid="{E0263BB3-4B13-4DFC-9DC6-C8E5BF01ED82}"/>
+    <hyperlink ref="E180:E189" r:id="rId298" display="https://insight.mdlz.com/p/" xr:uid="{65EFBE06-BFCB-4D33-9ED0-3AAFB1EF4140}"/>
+    <hyperlink ref="E174:E180" r:id="rId299" display="https://insight.mdlz.com/p/" xr:uid="{91B6F391-4447-4E46-83D1-A48B2271391F}"/>
+    <hyperlink ref="E180" r:id="rId300" xr:uid="{57ADF882-E9C2-4031-865D-13CBF9AA692E}"/>
+    <hyperlink ref="E181" r:id="rId301" xr:uid="{138E8275-ADE1-4AAD-A782-CDDF2D18E645}"/>
+    <hyperlink ref="E182" r:id="rId302" xr:uid="{7E9DF841-C05E-4C96-B62F-0BF1005CAEB3}"/>
+    <hyperlink ref="E183" r:id="rId303" location="frameworks-for-model-xai" xr:uid="{427C4DD7-A698-4C8E-B4CE-93596DD081F9}"/>
+    <hyperlink ref="E184" r:id="rId304" xr:uid="{6F3D1EA3-A8D3-486C-9CEE-55DE4A3BB7F5}"/>
+    <hyperlink ref="E185" r:id="rId305" xr:uid="{C99B0A4C-B705-4643-9C42-D6C8DCE81D6E}"/>
+    <hyperlink ref="E186" r:id="rId306" xr:uid="{A6ADAB43-85C5-4016-9FB9-28CC47A1AC71}"/>
+    <hyperlink ref="E187" r:id="rId307" xr:uid="{1AEC31E7-D921-43E3-B124-3799BACFF145}"/>
+    <hyperlink ref="E188" r:id="rId308" location="7-continuous-integration-ci" xr:uid="{9C65A458-C346-4E18-96EE-2B3DBDCFBA56}"/>
+    <hyperlink ref="E189" r:id="rId309" location="8-continuous-delivery" xr:uid="{932D40A7-D751-4E16-90F0-04E24FC3A0B2}"/>
+    <hyperlink ref="E191" r:id="rId310" xr:uid="{29F29713-B964-4741-8452-2DF1F5B0DE00}"/>
+    <hyperlink ref="E192" r:id="rId311" xr:uid="{3E680760-3849-4E9F-8E0C-C9488C7E3D70}"/>
+    <hyperlink ref="E193" r:id="rId312" xr:uid="{6BD1BF3C-199F-411C-867D-9765B6D62CEF}"/>
+    <hyperlink ref="E194" r:id="rId313" location="debt" xr:uid="{7DB13559-A9BF-4871-94B8-30FD20DAC041}"/>
+    <hyperlink ref="E195" r:id="rId314" xr:uid="{9B9EC260-8021-4EE6-9564-6DAC90B212A1}"/>
+    <hyperlink ref="E196" r:id="rId315" xr:uid="{7F24618A-017B-4C3C-9977-1162613F5368}"/>
+    <hyperlink ref="E197" r:id="rId316" xr:uid="{EEEB9C05-6CDB-40CC-8337-C6C88D338E11}"/>
+    <hyperlink ref="E198" r:id="rId317" xr:uid="{48CA2A86-E945-459C-B18D-8248FE0545D7}"/>
+    <hyperlink ref="E199" r:id="rId318" xr:uid="{96D681A6-66F0-47EC-AE25-0C2FFFCB23F1}"/>
+    <hyperlink ref="E201" r:id="rId319" xr:uid="{2688664A-C252-4849-AA40-FED3D669A7B2}"/>
+    <hyperlink ref="E200" r:id="rId320" xr:uid="{273A8154-28F2-47AD-9D4E-87EECB0C4BBD}"/>
+    <hyperlink ref="E202" r:id="rId321" xr:uid="{F3C1A791-8D5B-4A54-95A7-F562F06EB2C3}"/>
+    <hyperlink ref="E203" r:id="rId322" xr:uid="{E7E887A9-7FD5-48FB-B81A-36DB31B46619}"/>
+    <hyperlink ref="E204" r:id="rId323" location="workflow-performance-montoring" xr:uid="{594C4E25-2502-431B-B9DD-93C70766EF57}"/>
+    <hyperlink ref="E205" r:id="rId324" xr:uid="{E7902211-39BE-46EB-ACF8-DC755EFBBD66}"/>
+    <hyperlink ref="E206" r:id="rId325" xr:uid="{85F7A8A4-D2C0-446C-9731-05A4912036E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId255"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId326"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added questions for PMO and DevOps
</commit_message>
<xml_diff>
--- a/data/chatbot-1.xlsx
+++ b/data/chatbot-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJK3794\PycharmProjects\Datahub Chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D380BBD9-B669-470C-9573-32E954CA3244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BA2139-739B-4643-9651-E2D5DDC3B14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{CB1DE796-0A7F-4358-B0F5-62D7433C0693}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="621">
   <si>
     <t>Category</t>
   </si>
@@ -1728,6 +1728,183 @@
   </si>
   <si>
     <t xml:space="preserve">Model Experiments </t>
+  </si>
+  <si>
+    <t>MDS Project Mgmt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is Mondelez Portfolio (MSPO) Process </t>
+  </si>
+  <si>
+    <t>https://collaboration.mdlz.com/sites/PVRTeam</t>
+  </si>
+  <si>
+    <t>What is Mondelez Project Mgmt. Capability Framework</t>
+  </si>
+  <si>
+    <t>https://intranet.mdlz.com/sites/MIU/Pages/PMCDF.aspx</t>
+  </si>
+  <si>
+    <t>What is Mondelez Toll Gate Methodology for Project Delivery</t>
+  </si>
+  <si>
+    <t>https://collaboration.mdlz.com/sites/tollgatemethodology/Pages/HomePage.aspx</t>
+  </si>
+  <si>
+    <t>D&amp;A Project Mgmt.</t>
+  </si>
+  <si>
+    <t>Mondelez MDS D&amp;A General Onboarding</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/sites/usarise/Shared%20Documents/Forms/AllItems.aspx?FolderCTID=0x0120009687463DA2EB954FB59C1AE67439BA4C&amp;id=%2Fsites%2Fusarise%2FShared%20Documents%2FGeneral%2F00%2E%20Onboarding%2F01%2E%20MDS%2F10%2E%20Onboarding%20videos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where do I need to capture D&amp;A Project (Incl. Prototype) or Program Demand </t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/:x:/r/sites/ibsdataandanalytics/_layouts/15/Doc.aspx?sourcedoc=%7BB0793A6C-1CCA-4F8F-93B9-B1268718CB9D%7D&amp;file=Demand%20Tracker%20v.1.xlsx&amp;action=default&amp;mobileredirect=true</t>
+  </si>
+  <si>
+    <t>What is CMDL (Certified Master Data Lake)</t>
+  </si>
+  <si>
+    <t>https://collaboration.mdlz.com/sites/CMDLComms</t>
+  </si>
+  <si>
+    <t>Project Execution</t>
+  </si>
+  <si>
+    <t>Where can I find all Projects which are in Execution</t>
+  </si>
+  <si>
+    <t>Project Mgmt.</t>
+  </si>
+  <si>
+    <t>What is D&amp;A Operating Model for Project Delivery followed in LA region</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/sites/enterprisedataplatformteam/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=C7C4X1&amp;CID=8d0e24a9%2D7bea%2D46a6%2D9501%2D656778853926&amp;FolderCTID=0x012000C3AAEF24304CAA4B9AE73A9B852BAD69&amp;id=%2Fsites%2Fenterprisedataplatformteam%2FShared%20Documents%2FGeneral%2FD%26A%5FGovernance%20%26%20Methodology%2F1%2E%20D%26A%20Operating%20Model</t>
+  </si>
+  <si>
+    <t>What are deliverables to consider as part of D&amp;A Project Delivery</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/:b:/r/sites/enterprisedataplatformteam/Shared%20Documents/General/D%26A_Governance%20%26%20Methodology/1.%20D%26A%20Operating%20Model/Project%20Deliverables_by%20Phase.pdf?csf=1&amp;web=1&amp;e=whjcKp</t>
+  </si>
+  <si>
+    <t>How to move source code changes and prep for move to production?</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/sites/ibsdataandanalytics/Shared%20Documents/Production%20Change%20Control/01.%20Change%20Advisory%20Board/D&amp;A%20Calendar%20&amp;%20CAB%20-%20FAQ's.pptx?web=1</t>
+  </si>
+  <si>
+    <t>What is D&amp;A schedule for releasing changes in production environment?</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/sites/ibsdataandanalytics/Shared%20Documents/Production%20Change%20Control/01.%20Change%20Advisory%20Board/MDS%20D&amp;A%20Release%20Calendar_v1.xlsx?web=1</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is DevOps Engineer Practices </t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/:w:/r/sites/d4gvdevopscoe/_layouts/15/Doc.aspx?sourcedoc=%7BB405DD08-92FA-4C1A-B0D8-D05372A5E0A3%7D&amp;file=D4GV%20DevOps%20Handbook%202024.docx&amp;action=default&amp;mobileredirect=true</t>
+  </si>
+  <si>
+    <t>What is D&amp;A DevOps GitHub Branching Strategy and Process?</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/:w:/r/sites/ibsdataandanalytics/Shared%20Documents/Production%20Change%20Control/01.%20Change%20Advisory%20Board/CAB%20and%20GitHub%20code%20deployment%20process%20v2.docx?d=wbf81de9c93024ecb9c6cd27152081d0a&amp;csf=1&amp;web=1&amp;e=qopwwv</t>
+  </si>
+  <si>
+    <t>Test Mgmt.</t>
+  </si>
+  <si>
+    <t>What is D&amp;A Testing Framework</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/:p:/r/sites/d4gvdevopscoe/_layouts/15/Doc.aspx?sourcedoc=%7BABC5CA2C-F718-4163-828F-F18CF5B61AA5%7D&amp;file=Mondelez%20D%26A%20Testing%20Framework%20V2.0.pptx&amp;action=edit&amp;mobileredirect=true</t>
+  </si>
+  <si>
+    <t>What is D&amp;A Testing Handbook</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/:p:/r/sites/d4gvdevopscoe/_layouts/15/Doc.aspx?sourcedoc=%7B78F88548-641D-4497-9FDE-C895165FB6CE%7D&amp;file=D&amp;A%20Testing_Playbook.pptx=&amp;action=edit&amp;mobileredirect=true</t>
+  </si>
+  <si>
+    <t>How to use qTest for D&amp;A Project</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/:w:/r/sites/d4gvdevopscoe/_layouts/15/Doc.aspx?sourcedoc=%7B428FDC4F-ED90-41E5-AD5D-D8B4C53922CC%7D&amp;file=qTest%20User%20Manual.docx&amp;action=default&amp;mobileredirect=true</t>
+  </si>
+  <si>
+    <t>What is a Project Manager Handbook to be followed as best practices LA region</t>
+  </si>
+  <si>
+    <t>https://collaboration.mdlz.com/:w:/r/sites/LADataAnalytics/_layouts/15/guestaccess.aspx?share=EdBTILiOXkRLnjD_D7qeh4QBxpjsmZvjDmxtyooAaskaRg</t>
+  </si>
+  <si>
+    <t>https://partners.mdlz.com/:w:/r/sites/AMEADAWS/_layouts/15/doc2.aspx?sourcedoc=%7Bfa127fe4-126d-4545-a18d-60983f0d9927%7D&amp;action=edit&amp;wdPid=552febe9&amp;cid=4d38515f-afdf-4d61-a306-d25df37f26ae</t>
+  </si>
+  <si>
+    <t>What is a Project Manager Handbook to be followed as best practices AMEA region</t>
+  </si>
+  <si>
+    <t>MSPO Process</t>
+  </si>
+  <si>
+    <t>PMCDF</t>
+  </si>
+  <si>
+    <t>Toll Gate Methodology</t>
+  </si>
+  <si>
+    <t>D&amp;A General Onboarding</t>
+  </si>
+  <si>
+    <t>D&amp;A Demand Tracker</t>
+  </si>
+  <si>
+    <t>CMDL</t>
+  </si>
+  <si>
+    <t>Project List</t>
+  </si>
+  <si>
+    <t>D&amp;A Operating Model for Project Delivery</t>
+  </si>
+  <si>
+    <t>Project Manager Handbook LA</t>
+  </si>
+  <si>
+    <t>Project Manager Handbook AMEA</t>
+  </si>
+  <si>
+    <t>Project Deliverables</t>
+  </si>
+  <si>
+    <t>Production Change Control - FAQ</t>
+  </si>
+  <si>
+    <t>Production Change Control - Release Calendar</t>
+  </si>
+  <si>
+    <t>DevOps Handbook</t>
+  </si>
+  <si>
+    <t>Production Change Control - Deployment Process</t>
+  </si>
+  <si>
+    <t>D&amp;A Testing Framework</t>
+  </si>
+  <si>
+    <t>D&amp;A Testing Playbook</t>
+  </si>
+  <si>
+    <t>qTest</t>
   </si>
 </sst>
 </file>
@@ -1779,7 +1956,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1813,12 +1990,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1856,11 +2042,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2176,11 +2373,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}">
-  <dimension ref="A1:L206"/>
+  <dimension ref="A1:L224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F166" sqref="F166:F168"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F225" sqref="F225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5108,7 +5305,7 @@
       <c r="A141" t="s">
         <v>400</v>
       </c>
-      <c r="B141" s="17" t="s">
+      <c r="B141" s="19" t="s">
         <v>401</v>
       </c>
       <c r="C141" t="s">
@@ -5117,7 +5314,7 @@
       <c r="D141" t="s">
         <v>402</v>
       </c>
-      <c r="E141" s="18" t="s">
+      <c r="E141" s="20" t="s">
         <v>474</v>
       </c>
       <c r="F141" t="s">
@@ -5125,10 +5322,10 @@
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A142" s="17" t="s">
+      <c r="A142" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B142" s="17" t="s">
+      <c r="B142" s="19" t="s">
         <v>401</v>
       </c>
       <c r="C142" t="s">
@@ -5137,18 +5334,18 @@
       <c r="D142" t="s">
         <v>403</v>
       </c>
-      <c r="E142" s="19" t="s">
+      <c r="E142" s="21" t="s">
         <v>475</v>
       </c>
-      <c r="F142" s="17" t="s">
+      <c r="F142" s="19" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A143" s="17" t="s">
+      <c r="A143" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B143" s="17" t="s">
+      <c r="B143" s="19" t="s">
         <v>401</v>
       </c>
       <c r="C143" t="s">
@@ -5157,18 +5354,18 @@
       <c r="D143" t="s">
         <v>404</v>
       </c>
-      <c r="E143" s="18" t="s">
+      <c r="E143" s="20" t="s">
         <v>476</v>
       </c>
-      <c r="F143" s="17" t="s">
+      <c r="F143" s="19" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A144" s="17" t="s">
+      <c r="A144" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B144" s="17" t="s">
+      <c r="B144" s="19" t="s">
         <v>401</v>
       </c>
       <c r="C144" t="s">
@@ -5177,18 +5374,18 @@
       <c r="D144" t="s">
         <v>405</v>
       </c>
-      <c r="E144" s="18" t="s">
+      <c r="E144" s="20" t="s">
         <v>477</v>
       </c>
-      <c r="F144" s="17" t="s">
+      <c r="F144" s="19" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A145" s="17" t="s">
+      <c r="A145" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B145" s="17" t="s">
+      <c r="B145" s="19" t="s">
         <v>406</v>
       </c>
       <c r="C145" t="s">
@@ -5197,7 +5394,7 @@
       <c r="D145" t="s">
         <v>407</v>
       </c>
-      <c r="E145" s="18" t="s">
+      <c r="E145" s="20" t="s">
         <v>478</v>
       </c>
       <c r="F145" t="s">
@@ -5205,10 +5402,10 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A146" s="17" t="s">
+      <c r="A146" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B146" s="17" t="s">
+      <c r="B146" s="19" t="s">
         <v>406</v>
       </c>
       <c r="C146" t="s">
@@ -5217,18 +5414,18 @@
       <c r="D146" t="s">
         <v>408</v>
       </c>
-      <c r="E146" s="18" t="s">
+      <c r="E146" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="F146" s="17" t="s">
+      <c r="F146" s="19" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A147" s="17" t="s">
+      <c r="A147" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B147" s="17" t="s">
+      <c r="B147" s="19" t="s">
         <v>406</v>
       </c>
       <c r="C147" t="s">
@@ -5237,18 +5434,18 @@
       <c r="D147" t="s">
         <v>409</v>
       </c>
-      <c r="E147" s="18" t="s">
+      <c r="E147" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="F147" s="17" t="s">
+      <c r="F147" s="19" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A148" s="17" t="s">
+      <c r="A148" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B148" s="17" t="s">
+      <c r="B148" s="19" t="s">
         <v>406</v>
       </c>
       <c r="C148" t="s">
@@ -5257,18 +5454,18 @@
       <c r="D148" t="s">
         <v>410</v>
       </c>
-      <c r="E148" s="18" t="s">
+      <c r="E148" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="F148" s="17" t="s">
+      <c r="F148" s="19" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A149" s="17" t="s">
+      <c r="A149" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B149" s="17" t="s">
+      <c r="B149" s="19" t="s">
         <v>406</v>
       </c>
       <c r="C149" t="s">
@@ -5277,7 +5474,7 @@
       <c r="D149" t="s">
         <v>411</v>
       </c>
-      <c r="E149" s="18" t="s">
+      <c r="E149" s="20" t="s">
         <v>481</v>
       </c>
       <c r="F149" t="s">
@@ -5285,10 +5482,10 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A150" s="17" t="s">
+      <c r="A150" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B150" s="17" t="s">
+      <c r="B150" s="19" t="s">
         <v>406</v>
       </c>
       <c r="C150" t="s">
@@ -5297,18 +5494,18 @@
       <c r="D150" t="s">
         <v>412</v>
       </c>
-      <c r="E150" s="18" t="s">
+      <c r="E150" s="20" t="s">
         <v>482</v>
       </c>
-      <c r="F150" s="17" t="s">
+      <c r="F150" s="19" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A151" s="17" t="s">
+      <c r="A151" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B151" s="17" t="s">
+      <c r="B151" s="19" t="s">
         <v>413</v>
       </c>
       <c r="C151" t="s">
@@ -5317,18 +5514,18 @@
       <c r="D151" t="s">
         <v>414</v>
       </c>
-      <c r="E151" s="18" t="s">
+      <c r="E151" s="20" t="s">
         <v>483</v>
       </c>
-      <c r="F151" s="17" t="s">
+      <c r="F151" s="19" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A152" s="17" t="s">
+      <c r="A152" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B152" s="17" t="s">
+      <c r="B152" s="19" t="s">
         <v>413</v>
       </c>
       <c r="C152" t="s">
@@ -5337,18 +5534,18 @@
       <c r="D152" t="s">
         <v>415</v>
       </c>
-      <c r="E152" s="18" t="s">
+      <c r="E152" s="20" t="s">
         <v>483</v>
       </c>
-      <c r="F152" s="17" t="s">
+      <c r="F152" s="19" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A153" s="17" t="s">
+      <c r="A153" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B153" s="17" t="s">
+      <c r="B153" s="19" t="s">
         <v>413</v>
       </c>
       <c r="C153" t="s">
@@ -5357,18 +5554,18 @@
       <c r="D153" t="s">
         <v>416</v>
       </c>
-      <c r="E153" s="18" t="s">
+      <c r="E153" s="20" t="s">
         <v>483</v>
       </c>
-      <c r="F153" s="17" t="s">
+      <c r="F153" s="19" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A154" s="17" t="s">
+      <c r="A154" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B154" s="17" t="s">
+      <c r="B154" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C154" t="s">
@@ -5377,18 +5574,18 @@
       <c r="D154" t="s">
         <v>418</v>
       </c>
-      <c r="E154" s="18" t="s">
+      <c r="E154" s="20" t="s">
         <v>484</v>
       </c>
-      <c r="F154" s="17" t="s">
+      <c r="F154" s="19" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A155" s="17" t="s">
+      <c r="A155" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B155" s="17" t="s">
+      <c r="B155" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C155" t="s">
@@ -5397,18 +5594,18 @@
       <c r="D155" t="s">
         <v>419</v>
       </c>
-      <c r="E155" s="18" t="s">
+      <c r="E155" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="F155" s="17" t="s">
+      <c r="F155" s="19" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A156" s="17" t="s">
+      <c r="A156" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B156" s="17" t="s">
+      <c r="B156" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C156" t="s">
@@ -5417,18 +5614,18 @@
       <c r="D156" t="s">
         <v>420</v>
       </c>
-      <c r="E156" s="18" t="s">
+      <c r="E156" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="F156" s="17" t="s">
+      <c r="F156" s="19" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A157" s="17" t="s">
+      <c r="A157" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B157" s="17" t="s">
+      <c r="B157" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C157" t="s">
@@ -5437,18 +5634,18 @@
       <c r="D157" t="s">
         <v>421</v>
       </c>
-      <c r="E157" s="18" t="s">
+      <c r="E157" s="20" t="s">
         <v>486</v>
       </c>
-      <c r="F157" s="17" t="s">
+      <c r="F157" s="19" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A158" s="17" t="s">
+      <c r="A158" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B158" s="17" t="s">
+      <c r="B158" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C158" t="s">
@@ -5457,18 +5654,18 @@
       <c r="D158" t="s">
         <v>422</v>
       </c>
-      <c r="E158" s="18" t="s">
+      <c r="E158" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="F158" s="17" t="s">
+      <c r="F158" s="19" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A159" s="17" t="s">
+      <c r="A159" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B159" s="17" t="s">
+      <c r="B159" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C159" t="s">
@@ -5477,7 +5674,7 @@
       <c r="D159" t="s">
         <v>423</v>
       </c>
-      <c r="E159" s="18" t="s">
+      <c r="E159" s="20" t="s">
         <v>487</v>
       </c>
       <c r="F159" t="s">
@@ -5485,10 +5682,10 @@
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A160" s="17" t="s">
+      <c r="A160" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B160" s="17" t="s">
+      <c r="B160" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C160" t="s">
@@ -5497,18 +5694,18 @@
       <c r="D160" t="s">
         <v>424</v>
       </c>
-      <c r="E160" s="18" t="s">
+      <c r="E160" s="20" t="s">
         <v>488</v>
       </c>
-      <c r="F160" s="17" t="s">
+      <c r="F160" s="19" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A161" s="17" t="s">
+      <c r="A161" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B161" s="17" t="s">
+      <c r="B161" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C161" t="s">
@@ -5517,18 +5714,18 @@
       <c r="D161" t="s">
         <v>425</v>
       </c>
-      <c r="E161" s="18" t="s">
+      <c r="E161" s="20" t="s">
         <v>487</v>
       </c>
-      <c r="F161" s="17" t="s">
+      <c r="F161" s="19" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A162" s="17" t="s">
+      <c r="A162" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B162" s="17" t="s">
+      <c r="B162" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C162" t="s">
@@ -5537,7 +5734,7 @@
       <c r="D162" t="s">
         <v>426</v>
       </c>
-      <c r="E162" s="18" t="s">
+      <c r="E162" s="20" t="s">
         <v>489</v>
       </c>
       <c r="F162" t="s">
@@ -5545,10 +5742,10 @@
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A163" s="17" t="s">
+      <c r="A163" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B163" s="17" t="s">
+      <c r="B163" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C163" t="s">
@@ -5557,7 +5754,7 @@
       <c r="D163" t="s">
         <v>427</v>
       </c>
-      <c r="E163" s="18" t="s">
+      <c r="E163" s="20" t="s">
         <v>490</v>
       </c>
       <c r="F163" t="s">
@@ -5565,10 +5762,10 @@
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A164" s="17" t="s">
+      <c r="A164" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B164" s="17" t="s">
+      <c r="B164" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C164" t="s">
@@ -5577,18 +5774,18 @@
       <c r="D164" t="s">
         <v>428</v>
       </c>
-      <c r="E164" s="18" t="s">
+      <c r="E164" s="20" t="s">
         <v>491</v>
       </c>
-      <c r="F164" s="17" t="s">
+      <c r="F164" s="19" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A165" s="17" t="s">
+      <c r="A165" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B165" s="17" t="s">
+      <c r="B165" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C165" t="s">
@@ -5597,18 +5794,18 @@
       <c r="D165" t="s">
         <v>429</v>
       </c>
-      <c r="E165" s="18" t="s">
+      <c r="E165" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="F165" s="17" t="s">
+      <c r="F165" s="19" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A166" s="17" t="s">
+      <c r="A166" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B166" s="17" t="s">
+      <c r="B166" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C166" t="s">
@@ -5617,18 +5814,18 @@
       <c r="D166" t="s">
         <v>430</v>
       </c>
-      <c r="E166" s="18" t="s">
+      <c r="E166" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="F166" s="17" t="s">
+      <c r="F166" s="19" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A167" s="17" t="s">
+      <c r="A167" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B167" s="17" t="s">
+      <c r="B167" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C167" t="s">
@@ -5637,18 +5834,18 @@
       <c r="D167" t="s">
         <v>431</v>
       </c>
-      <c r="E167" s="18" t="s">
+      <c r="E167" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="F167" s="17" t="s">
+      <c r="F167" s="19" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A168" s="17" t="s">
+      <c r="A168" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B168" s="17" t="s">
+      <c r="B168" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C168" t="s">
@@ -5657,18 +5854,18 @@
       <c r="D168" t="s">
         <v>432</v>
       </c>
-      <c r="E168" s="18" t="s">
+      <c r="E168" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="F168" s="17" t="s">
+      <c r="F168" s="19" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A169" s="17" t="s">
+      <c r="A169" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B169" s="17" t="s">
+      <c r="B169" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C169" t="s">
@@ -5677,18 +5874,18 @@
       <c r="D169" t="s">
         <v>433</v>
       </c>
-      <c r="E169" s="18" t="s">
+      <c r="E169" s="20" t="s">
         <v>493</v>
       </c>
-      <c r="F169" s="17" t="s">
+      <c r="F169" s="19" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A170" s="17" t="s">
+      <c r="A170" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B170" s="17" t="s">
+      <c r="B170" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C170" t="s">
@@ -5697,18 +5894,18 @@
       <c r="D170" t="s">
         <v>434</v>
       </c>
-      <c r="E170" s="18" t="s">
+      <c r="E170" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="F170" s="17" t="s">
+      <c r="F170" s="19" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A171" s="17" t="s">
+      <c r="A171" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B171" s="17" t="s">
+      <c r="B171" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C171" t="s">
@@ -5717,18 +5914,18 @@
       <c r="D171" t="s">
         <v>435</v>
       </c>
-      <c r="E171" s="18" t="s">
+      <c r="E171" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="F171" s="17" t="s">
+      <c r="F171" s="19" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A172" s="17" t="s">
+      <c r="A172" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B172" s="17" t="s">
+      <c r="B172" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C172" t="s">
@@ -5737,18 +5934,18 @@
       <c r="D172" t="s">
         <v>436</v>
       </c>
-      <c r="E172" s="18" t="s">
+      <c r="E172" s="20" t="s">
         <v>495</v>
       </c>
-      <c r="F172" s="17" t="s">
+      <c r="F172" s="19" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A173" s="17" t="s">
+      <c r="A173" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B173" s="17" t="s">
+      <c r="B173" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C173" t="s">
@@ -5757,18 +5954,18 @@
       <c r="D173" t="s">
         <v>437</v>
       </c>
-      <c r="E173" s="18" t="s">
+      <c r="E173" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="F173" s="17" t="s">
+      <c r="F173" s="19" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A174" s="17" t="s">
+      <c r="A174" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B174" s="17" t="s">
+      <c r="B174" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C174" t="s">
@@ -5777,18 +5974,18 @@
       <c r="D174" t="s">
         <v>438</v>
       </c>
-      <c r="E174" s="18" t="s">
+      <c r="E174" s="20" t="s">
         <v>496</v>
       </c>
-      <c r="F174" s="17" t="s">
+      <c r="F174" s="19" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A175" s="17" t="s">
+      <c r="A175" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B175" s="17" t="s">
+      <c r="B175" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C175" t="s">
@@ -5797,18 +5994,18 @@
       <c r="D175" t="s">
         <v>439</v>
       </c>
-      <c r="E175" s="18" t="s">
+      <c r="E175" s="20" t="s">
         <v>497</v>
       </c>
-      <c r="F175" s="17" t="s">
+      <c r="F175" s="19" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A176" s="17" t="s">
+      <c r="A176" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B176" s="17" t="s">
+      <c r="B176" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C176" t="s">
@@ -5817,18 +6014,18 @@
       <c r="D176" t="s">
         <v>440</v>
       </c>
-      <c r="E176" s="18" t="s">
+      <c r="E176" s="20" t="s">
         <v>498</v>
       </c>
-      <c r="F176" s="17" t="s">
+      <c r="F176" s="19" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A177" s="17" t="s">
+      <c r="A177" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B177" s="17" t="s">
+      <c r="B177" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C177" t="s">
@@ -5837,18 +6034,18 @@
       <c r="D177" t="s">
         <v>441</v>
       </c>
-      <c r="E177" s="18" t="s">
+      <c r="E177" s="20" t="s">
         <v>496</v>
       </c>
-      <c r="F177" s="17" t="s">
+      <c r="F177" s="19" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A178" s="17" t="s">
+      <c r="A178" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B178" s="17" t="s">
+      <c r="B178" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C178" t="s">
@@ -5857,18 +6054,18 @@
       <c r="D178" t="s">
         <v>442</v>
       </c>
-      <c r="E178" s="18" t="s">
+      <c r="E178" s="20" t="s">
         <v>499</v>
       </c>
-      <c r="F178" s="17" t="s">
+      <c r="F178" s="19" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A179" s="17" t="s">
+      <c r="A179" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B179" s="17" t="s">
+      <c r="B179" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C179" t="s">
@@ -5877,18 +6074,18 @@
       <c r="D179" t="s">
         <v>443</v>
       </c>
-      <c r="E179" s="18" t="s">
+      <c r="E179" s="20" t="s">
         <v>499</v>
       </c>
-      <c r="F179" s="17" t="s">
+      <c r="F179" s="19" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A180" s="17" t="s">
+      <c r="A180" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B180" s="17" t="s">
+      <c r="B180" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C180" t="s">
@@ -5897,18 +6094,18 @@
       <c r="D180" t="s">
         <v>444</v>
       </c>
-      <c r="E180" s="18" t="s">
+      <c r="E180" s="20" t="s">
         <v>499</v>
       </c>
-      <c r="F180" s="17" t="s">
+      <c r="F180" s="19" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A181" s="17" t="s">
+      <c r="A181" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B181" s="17" t="s">
+      <c r="B181" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C181" t="s">
@@ -5917,18 +6114,18 @@
       <c r="D181" t="s">
         <v>445</v>
       </c>
-      <c r="E181" s="18" t="s">
+      <c r="E181" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="F181" s="17" t="s">
+      <c r="F181" s="19" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A182" s="17" t="s">
+      <c r="A182" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B182" s="17" t="s">
+      <c r="B182" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C182" t="s">
@@ -5937,18 +6134,18 @@
       <c r="D182" t="s">
         <v>446</v>
       </c>
-      <c r="E182" s="18" t="s">
+      <c r="E182" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="F182" s="17" t="s">
+      <c r="F182" s="19" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A183" s="17" t="s">
+      <c r="A183" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B183" s="17" t="s">
+      <c r="B183" s="19" t="s">
         <v>417</v>
       </c>
       <c r="C183" t="s">
@@ -5957,18 +6154,18 @@
       <c r="D183" t="s">
         <v>447</v>
       </c>
-      <c r="E183" s="18" t="s">
+      <c r="E183" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="F183" s="17" t="s">
+      <c r="F183" s="19" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A184" s="17" t="s">
+      <c r="A184" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B184" s="17" t="s">
+      <c r="B184" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C184" t="s">
@@ -5977,18 +6174,18 @@
       <c r="D184" t="s">
         <v>449</v>
       </c>
-      <c r="E184" s="18" t="s">
+      <c r="E184" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="F184" s="17" t="s">
+      <c r="F184" s="19" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A185" s="17" t="s">
+      <c r="A185" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B185" s="17" t="s">
+      <c r="B185" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C185" t="s">
@@ -5997,18 +6194,18 @@
       <c r="D185" t="s">
         <v>450</v>
       </c>
-      <c r="E185" s="18" t="s">
+      <c r="E185" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="F185" s="17" t="s">
+      <c r="F185" s="19" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A186" s="17" t="s">
+      <c r="A186" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B186" s="17" t="s">
+      <c r="B186" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C186" t="s">
@@ -6017,18 +6214,18 @@
       <c r="D186" t="s">
         <v>451</v>
       </c>
-      <c r="E186" s="18" t="s">
+      <c r="E186" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="F186" s="17" t="s">
+      <c r="F186" s="19" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A187" s="17" t="s">
+      <c r="A187" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B187" s="17" t="s">
+      <c r="B187" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C187" t="s">
@@ -6037,18 +6234,18 @@
       <c r="D187" t="s">
         <v>452</v>
       </c>
-      <c r="E187" s="18" t="s">
+      <c r="E187" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="F187" s="17" t="s">
+      <c r="F187" s="19" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A188" s="17" t="s">
+      <c r="A188" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B188" s="17" t="s">
+      <c r="B188" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C188" t="s">
@@ -6057,18 +6254,18 @@
       <c r="D188" t="s">
         <v>453</v>
       </c>
-      <c r="E188" s="18" t="s">
+      <c r="E188" s="20" t="s">
         <v>503</v>
       </c>
-      <c r="F188" s="17" t="s">
+      <c r="F188" s="19" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A189" s="17" t="s">
+      <c r="A189" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B189" s="17" t="s">
+      <c r="B189" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C189" t="s">
@@ -6077,18 +6274,18 @@
       <c r="D189" t="s">
         <v>454</v>
       </c>
-      <c r="E189" s="18" t="s">
+      <c r="E189" s="20" t="s">
         <v>504</v>
       </c>
-      <c r="F189" s="17" t="s">
+      <c r="F189" s="19" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A190" s="17" t="s">
+      <c r="A190" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B190" s="17" t="s">
+      <c r="B190" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C190" t="s">
@@ -6097,18 +6294,18 @@
       <c r="D190" t="s">
         <v>455</v>
       </c>
-      <c r="E190" s="18" t="s">
+      <c r="E190" s="20" t="s">
         <v>505</v>
       </c>
-      <c r="F190" s="17" t="s">
+      <c r="F190" s="19" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A191" s="17" t="s">
+      <c r="A191" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B191" s="17" t="s">
+      <c r="B191" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C191" t="s">
@@ -6117,18 +6314,18 @@
       <c r="D191" t="s">
         <v>456</v>
       </c>
-      <c r="E191" s="18" t="s">
+      <c r="E191" s="20" t="s">
         <v>506</v>
       </c>
-      <c r="F191" s="17" t="s">
+      <c r="F191" s="19" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A192" s="17" t="s">
+      <c r="A192" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B192" s="17" t="s">
+      <c r="B192" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C192" t="s">
@@ -6137,18 +6334,18 @@
       <c r="D192" t="s">
         <v>457</v>
       </c>
-      <c r="E192" s="18" t="s">
+      <c r="E192" s="20" t="s">
         <v>507</v>
       </c>
-      <c r="F192" s="17" t="s">
+      <c r="F192" s="19" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A193" s="17" t="s">
+      <c r="A193" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B193" s="17" t="s">
+      <c r="B193" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C193" t="s">
@@ -6157,18 +6354,18 @@
       <c r="D193" t="s">
         <v>458</v>
       </c>
-      <c r="E193" s="18" t="s">
+      <c r="E193" s="20" t="s">
         <v>507</v>
       </c>
-      <c r="F193" s="17" t="s">
+      <c r="F193" s="19" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A194" s="17" t="s">
+      <c r="A194" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B194" s="17" t="s">
+      <c r="B194" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C194" t="s">
@@ -6177,18 +6374,18 @@
       <c r="D194" t="s">
         <v>459</v>
       </c>
-      <c r="E194" s="18" t="s">
+      <c r="E194" s="20" t="s">
         <v>508</v>
       </c>
-      <c r="F194" s="17" t="s">
+      <c r="F194" s="19" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A195" s="17" t="s">
+      <c r="A195" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B195" s="17" t="s">
+      <c r="B195" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C195" t="s">
@@ -6197,18 +6394,18 @@
       <c r="D195" t="s">
         <v>460</v>
       </c>
-      <c r="E195" s="18" t="s">
+      <c r="E195" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="F195" s="17" t="s">
+      <c r="F195" s="19" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A196" s="17" t="s">
+      <c r="A196" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B196" s="17" t="s">
+      <c r="B196" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C196" t="s">
@@ -6217,18 +6414,18 @@
       <c r="D196" t="s">
         <v>461</v>
       </c>
-      <c r="E196" s="18" t="s">
+      <c r="E196" s="20" t="s">
         <v>510</v>
       </c>
-      <c r="F196" s="17" t="s">
+      <c r="F196" s="19" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A197" s="17" t="s">
+      <c r="A197" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B197" s="17" t="s">
+      <c r="B197" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C197" t="s">
@@ -6237,18 +6434,18 @@
       <c r="D197" t="s">
         <v>462</v>
       </c>
-      <c r="E197" s="18" t="s">
+      <c r="E197" s="20" t="s">
         <v>510</v>
       </c>
-      <c r="F197" s="17" t="s">
+      <c r="F197" s="19" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A198" s="17" t="s">
+      <c r="A198" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B198" s="17" t="s">
+      <c r="B198" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C198" t="s">
@@ -6257,18 +6454,18 @@
       <c r="D198" t="s">
         <v>463</v>
       </c>
-      <c r="E198" s="18" t="s">
+      <c r="E198" s="20" t="s">
         <v>511</v>
       </c>
-      <c r="F198" s="17" t="s">
+      <c r="F198" s="19" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A199" s="17" t="s">
+      <c r="A199" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B199" s="17" t="s">
+      <c r="B199" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C199" t="s">
@@ -6277,18 +6474,18 @@
       <c r="D199" t="s">
         <v>464</v>
       </c>
-      <c r="E199" s="18" t="s">
+      <c r="E199" s="20" t="s">
         <v>511</v>
       </c>
-      <c r="F199" s="17" t="s">
+      <c r="F199" s="19" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A200" s="17" t="s">
+      <c r="A200" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B200" s="17" t="s">
+      <c r="B200" s="19" t="s">
         <v>448</v>
       </c>
       <c r="C200" t="s">
@@ -6297,18 +6494,18 @@
       <c r="D200" t="s">
         <v>465</v>
       </c>
-      <c r="E200" s="18" t="s">
+      <c r="E200" s="20" t="s">
         <v>512</v>
       </c>
-      <c r="F200" s="17" t="s">
+      <c r="F200" s="19" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A201" s="17" t="s">
+      <c r="A201" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B201" s="17" t="s">
+      <c r="B201" s="19" t="s">
         <v>466</v>
       </c>
       <c r="C201" t="s">
@@ -6317,18 +6514,18 @@
       <c r="D201" t="s">
         <v>467</v>
       </c>
-      <c r="E201" s="18" t="s">
+      <c r="E201" s="20" t="s">
         <v>512</v>
       </c>
-      <c r="F201" s="17" t="s">
+      <c r="F201" s="19" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A202" s="17" t="s">
+      <c r="A202" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B202" s="17" t="s">
+      <c r="B202" s="19" t="s">
         <v>466</v>
       </c>
       <c r="C202" t="s">
@@ -6337,18 +6534,18 @@
       <c r="D202" t="s">
         <v>468</v>
       </c>
-      <c r="E202" s="18" t="s">
+      <c r="E202" s="20" t="s">
         <v>513</v>
       </c>
-      <c r="F202" s="17" t="s">
+      <c r="F202" s="19" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A203" s="17" t="s">
+      <c r="A203" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B203" s="17" t="s">
+      <c r="B203" s="19" t="s">
         <v>466</v>
       </c>
       <c r="C203" t="s">
@@ -6357,18 +6554,18 @@
       <c r="D203" t="s">
         <v>469</v>
       </c>
-      <c r="E203" s="18" t="s">
+      <c r="E203" s="20" t="s">
         <v>513</v>
       </c>
-      <c r="F203" s="17" t="s">
+      <c r="F203" s="19" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A204" s="17" t="s">
+      <c r="A204" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B204" s="17" t="s">
+      <c r="B204" s="19" t="s">
         <v>466</v>
       </c>
       <c r="C204" t="s">
@@ -6377,18 +6574,18 @@
       <c r="D204" t="s">
         <v>470</v>
       </c>
-      <c r="E204" s="18" t="s">
+      <c r="E204" s="20" t="s">
         <v>514</v>
       </c>
-      <c r="F204" s="17" t="s">
+      <c r="F204" s="19" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A205" s="17" t="s">
+      <c r="A205" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B205" s="17" t="s">
+      <c r="B205" s="19" t="s">
         <v>413</v>
       </c>
       <c r="C205" t="s">
@@ -6397,18 +6594,18 @@
       <c r="D205" t="s">
         <v>471</v>
       </c>
-      <c r="E205" s="18" t="s">
+      <c r="E205" s="20" t="s">
         <v>515</v>
       </c>
-      <c r="F205" s="17" t="s">
+      <c r="F205" s="19" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A206" s="17" t="s">
+      <c r="A206" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B206" s="17" t="s">
+      <c r="B206" s="19" t="s">
         <v>472</v>
       </c>
       <c r="C206" t="s">
@@ -6417,11 +6614,371 @@
       <c r="D206" t="s">
         <v>473</v>
       </c>
-      <c r="E206" s="18" t="s">
+      <c r="E206" s="20" t="s">
         <v>516</v>
       </c>
-      <c r="F206" s="17" t="s">
+      <c r="F206" s="19" t="s">
         <v>530</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A207" s="25" t="s">
+        <v>562</v>
+      </c>
+      <c r="B207" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C207" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D207" s="23" t="s">
+        <v>563</v>
+      </c>
+      <c r="E207" s="24" t="s">
+        <v>564</v>
+      </c>
+      <c r="F207" s="17" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A208" s="25" t="s">
+        <v>562</v>
+      </c>
+      <c r="B208" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C208" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D208" s="23" t="s">
+        <v>565</v>
+      </c>
+      <c r="E208" s="24" t="s">
+        <v>566</v>
+      </c>
+      <c r="F208" s="18" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A209" s="25" t="s">
+        <v>562</v>
+      </c>
+      <c r="B209" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C209" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D209" s="23" t="s">
+        <v>567</v>
+      </c>
+      <c r="E209" s="24" t="s">
+        <v>568</v>
+      </c>
+      <c r="F209" s="18" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A210" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B210" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C210" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D210" s="23" t="s">
+        <v>570</v>
+      </c>
+      <c r="E210" s="24" t="s">
+        <v>571</v>
+      </c>
+      <c r="F210" s="18" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A211" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B211" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C211" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D211" s="23" t="s">
+        <v>572</v>
+      </c>
+      <c r="E211" s="24" t="s">
+        <v>573</v>
+      </c>
+      <c r="F211" s="18" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A212" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B212" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C212" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D212" s="23" t="s">
+        <v>574</v>
+      </c>
+      <c r="E212" s="24" t="s">
+        <v>575</v>
+      </c>
+      <c r="F212" s="18" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A213" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B213" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C213" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D213" s="23" t="s">
+        <v>577</v>
+      </c>
+      <c r="E213" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="F213" s="18" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A214" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B214" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C214" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="D214" s="23" t="s">
+        <v>579</v>
+      </c>
+      <c r="E214" s="24" t="s">
+        <v>580</v>
+      </c>
+      <c r="F214" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A215" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B215" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C215" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="D215" s="23" t="s">
+        <v>599</v>
+      </c>
+      <c r="E215" s="24" t="s">
+        <v>600</v>
+      </c>
+      <c r="F215" s="26" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A216" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B216" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C216" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="D216" s="23" t="s">
+        <v>602</v>
+      </c>
+      <c r="E216" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="F216" s="18" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A217" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B217" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C217" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="D217" s="25" t="s">
+        <v>581</v>
+      </c>
+      <c r="E217" s="24" t="s">
+        <v>582</v>
+      </c>
+      <c r="F217" s="18" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A218" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B218" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C218" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="D218" s="25" t="s">
+        <v>583</v>
+      </c>
+      <c r="E218" s="24" t="s">
+        <v>584</v>
+      </c>
+      <c r="F218" s="18" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A219" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B219" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C219" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="D219" s="25" t="s">
+        <v>585</v>
+      </c>
+      <c r="E219" s="24" t="s">
+        <v>586</v>
+      </c>
+      <c r="F219" s="18" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A220" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B220" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C220" s="25" t="s">
+        <v>587</v>
+      </c>
+      <c r="D220" s="23" t="s">
+        <v>588</v>
+      </c>
+      <c r="E220" s="24" t="s">
+        <v>589</v>
+      </c>
+      <c r="F220" s="18" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A221" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B221" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C221" s="25" t="s">
+        <v>587</v>
+      </c>
+      <c r="D221" s="23" t="s">
+        <v>590</v>
+      </c>
+      <c r="E221" s="24" t="s">
+        <v>591</v>
+      </c>
+      <c r="F221" s="18" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A222" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B222" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C222" s="25" t="s">
+        <v>592</v>
+      </c>
+      <c r="D222" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="E222" s="24" t="s">
+        <v>594</v>
+      </c>
+      <c r="F222" s="18" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A223" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B223" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C223" s="25" t="s">
+        <v>592</v>
+      </c>
+      <c r="D223" s="23" t="s">
+        <v>595</v>
+      </c>
+      <c r="E223" s="24" t="s">
+        <v>596</v>
+      </c>
+      <c r="F223" s="18" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A224" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B224" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C224" s="25" t="s">
+        <v>592</v>
+      </c>
+      <c r="D224" s="25" t="s">
+        <v>597</v>
+      </c>
+      <c r="E224" s="24" t="s">
+        <v>598</v>
+      </c>
+      <c r="F224" s="18" t="s">
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -6752,9 +7309,29 @@
     <hyperlink ref="E204" r:id="rId323" location="workflow-performance-montoring" xr:uid="{594C4E25-2502-431B-B9DD-93C70766EF57}"/>
     <hyperlink ref="E205" r:id="rId324" xr:uid="{E7902211-39BE-46EB-ACF8-DC755EFBBD66}"/>
     <hyperlink ref="E206" r:id="rId325" xr:uid="{85F7A8A4-D2C0-446C-9731-05A4912036E2}"/>
+    <hyperlink ref="E207" r:id="rId326" xr:uid="{D60C86CA-DE10-42CE-B8BC-016EF3BEC45B}"/>
+    <hyperlink ref="E208" r:id="rId327" xr:uid="{B88A28D6-2776-4E6D-8E8F-0CAF4F45B6D9}"/>
+    <hyperlink ref="E209" r:id="rId328" xr:uid="{2B6CB2D2-7818-4692-BB5E-1D4D13590EC8}"/>
+    <hyperlink ref="E210" r:id="rId329" xr:uid="{AF6C72DF-4FBD-4CB0-9D30-4F887C820BC6}"/>
+    <hyperlink ref="E211" r:id="rId330" xr:uid="{B5DB5909-CAE3-41DE-8FAA-2BE9405FE89D}"/>
+    <hyperlink ref="E212" r:id="rId331" xr:uid="{EB971EED-5319-4B5A-866B-6272F1177031}"/>
+    <hyperlink ref="E213" r:id="rId332" xr:uid="{572B6EAD-FA78-4215-8917-A3C00D5ABFE0}"/>
+    <hyperlink ref="E214" r:id="rId333" display="https://teams.mdlz.com/sites/enterprisedataplatformteam/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=C7C4X1&amp;CID=8d0e24a9%2D7bea%2D46a6%2D9501%2D656778853926&amp;FolderCTID=0x012000C3AAEF24304CAA4B9AE73A9B852BAD69&amp;id=%2Fsites%2Fenterprisedataplatformteam%2FShared%20Documents%2FGeneral%2FD%26A%5FGovernance%20%26%20Methodology%2F1%2E%20D%26A%20Operating%20Model" xr:uid="{68BBCE6F-8DA7-464D-950F-BC16B0FF571C}"/>
+    <hyperlink ref="E220" r:id="rId334" xr:uid="{4CB97E97-7749-4435-94AD-D2868D458F68}"/>
+    <hyperlink ref="E222" r:id="rId335" xr:uid="{A474367E-A77D-4DEF-85B7-EEA70951388E}"/>
+    <hyperlink ref="E223" r:id="rId336" xr:uid="{68A144C1-9301-4982-9D52-3E933824C145}"/>
+    <hyperlink ref="E224" r:id="rId337" xr:uid="{A289F92F-FDC4-4101-860D-E87FC724D2BF}"/>
+    <hyperlink ref="E217" r:id="rId338" xr:uid="{7FE505FE-5854-4EEC-9F18-EC57B446CAB8}"/>
+    <hyperlink ref="E218" r:id="rId339" xr:uid="{FAF735B2-76DF-4822-819D-3825B225638C}"/>
+    <hyperlink ref="E219" r:id="rId340" xr:uid="{BFCB53CB-917E-4F45-9B9B-5CF694A05B23}"/>
+    <hyperlink ref="E221" r:id="rId341" xr:uid="{60C77EDA-E2FD-4625-89AC-626B3B109939}"/>
+    <hyperlink ref="E216" r:id="rId342" xr:uid="{9B7F4E7B-88C8-478A-BA8C-0835ECDAC49D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId326"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId343"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Mondelez International Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -6936,6 +7513,9 @@
     <hyperlink ref="C4" r:id="rId20" xr:uid="{1F0BA727-989D-43C6-B103-92A2D5D31CEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Mondelez International Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -8621,5 +9201,14 @@
     <hyperlink ref="E93" r:id="rId88" display="../../../../:b:/s/dadocumentrepository/EaCM77nIUIhAspPUFy-P0UsBIEVBLHGi1AZ9QLbrrBrLcA?e=vjl2Jr" xr:uid="{7DDCDDE9-71A9-4A16-B9B4-82C685432B2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Mondelez International Internal</oddFooter>
+  </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{a9324442-4656-4fca-b26e-099b64ea741e}" enabled="1" method="Standard" siteId="{18a01ad8-9727-498a-a47d-17374c6fd9f7}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Changed category grouping and renamed title
</commit_message>
<xml_diff>
--- a/data/chatbot-1.xlsx
+++ b/data/chatbot-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJK3794\PycharmProjects\Datahub Chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BA2139-739B-4643-9651-E2D5DDC3B14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989A3AE4-CB6E-41A1-8076-EC91245F1CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{CB1DE796-0A7F-4358-B0F5-62D7433C0693}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FAQ!$A$1:$A$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$224</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentManualCount="16"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="619">
   <si>
     <t>Category</t>
   </si>
@@ -905,9 +905,6 @@
     <t>Demand Intake</t>
   </si>
   <si>
-    <t>PMO</t>
-  </si>
-  <si>
     <t>ACE</t>
   </si>
   <si>
@@ -1728,9 +1725,6 @@
   </si>
   <si>
     <t xml:space="preserve">Model Experiments </t>
-  </si>
-  <si>
-    <t>MDS Project Mgmt.</t>
   </si>
   <si>
     <t xml:space="preserve">What is Mondelez Portfolio (MSPO) Process </t>
@@ -2376,8 +2370,8 @@
   <dimension ref="A1:L224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F225" sqref="F225"/>
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105:A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4361,7 +4355,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>268</v>
       </c>
@@ -4521,7 +4515,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>268</v>
       </c>
@@ -4582,8 +4576,8 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>287</v>
+      <c r="A105" s="25" t="s">
+        <v>567</v>
       </c>
       <c r="B105" s="13" t="s">
         <v>259</v>
@@ -4602,8 +4596,8 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>287</v>
+      <c r="A106" s="25" t="s">
+        <v>567</v>
       </c>
       <c r="B106" t="s">
         <v>259</v>
@@ -4622,8 +4616,8 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
-        <v>287</v>
+      <c r="A107" s="25" t="s">
+        <v>567</v>
       </c>
       <c r="B107" s="14" t="s">
         <v>261</v>
@@ -4643,7 +4637,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B108" s="14" t="s">
         <v>264</v>
@@ -4663,7 +4657,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B109" s="14" t="s">
         <v>265</v>
@@ -4683,67 +4677,67 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>362</v>
+      </c>
+      <c r="B110" s="16" t="s">
         <v>363</v>
       </c>
-      <c r="B110" s="16" t="s">
-        <v>364</v>
-      </c>
       <c r="C110" s="16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D110" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
+        <v>362</v>
+      </c>
+      <c r="B111" s="16" t="s">
         <v>363</v>
       </c>
-      <c r="B111" s="16" t="s">
-        <v>364</v>
-      </c>
       <c r="C111" s="16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D111" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F111" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
+        <v>362</v>
+      </c>
+      <c r="B112" s="16" t="s">
         <v>363</v>
       </c>
-      <c r="B112" s="16" t="s">
-        <v>364</v>
-      </c>
       <c r="C112" s="16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D112" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F112" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B113" s="16" t="s">
         <v>286</v>
@@ -4752,18 +4746,18 @@
         <v>286</v>
       </c>
       <c r="D113" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F113" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B114" s="16" t="s">
         <v>286</v>
@@ -4772,18 +4766,18 @@
         <v>286</v>
       </c>
       <c r="D114" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F114" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B115" s="16" t="s">
         <v>286</v>
@@ -4792,1838 +4786,1838 @@
         <v>286</v>
       </c>
       <c r="D115" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F115" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B116" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C116" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F116" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B117" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C117" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D117" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F117" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B118" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C118" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D118" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F118" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B119" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C119" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F119" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B120" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C120" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D120" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F120" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B121" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C121" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D121" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F121" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B122" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C122" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D122" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F122" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B123" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C123" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D123" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F123" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B124" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C124" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D124" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F124" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B125" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C125" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D125" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F125" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B126" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C126" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D126" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F126" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B127" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C127" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D127" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F127" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B128" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C128" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D128" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F128" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B129" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C129" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D129" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F129" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B130" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C130" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D130" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F130" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B131" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C131" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D131" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F131" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B132" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C132" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D132" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F132" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B133" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C133" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D133" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F133" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B134" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C134" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D134" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F134" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B135" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C135" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D135" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F135" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B136" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C136" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D136" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F136" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B137" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C137" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D137" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F137" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B138" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C138" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D138" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F138" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B139" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C139" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D139" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F139" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B140" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C140" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D140" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F140" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
+        <v>399</v>
+      </c>
+      <c r="B141" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B141" s="19" t="s">
+      <c r="C141" t="s">
+        <v>400</v>
+      </c>
+      <c r="D141" t="s">
         <v>401</v>
       </c>
-      <c r="C141" t="s">
-        <v>401</v>
-      </c>
-      <c r="D141" t="s">
+      <c r="E141" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="F141" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A142" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="B142" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="C142" t="s">
+        <v>400</v>
+      </c>
+      <c r="D142" t="s">
         <v>402</v>
       </c>
-      <c r="E141" s="20" t="s">
+      <c r="E142" s="21" t="s">
         <v>474</v>
       </c>
-      <c r="F141" t="s">
+      <c r="F142" s="19" t="s">
         <v>540</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A142" s="19" t="s">
-        <v>400</v>
-      </c>
-      <c r="B142" s="19" t="s">
-        <v>401</v>
-      </c>
-      <c r="C142" t="s">
-        <v>401</v>
-      </c>
-      <c r="D142" t="s">
-        <v>403</v>
-      </c>
-      <c r="E142" s="21" t="s">
-        <v>475</v>
-      </c>
-      <c r="F142" s="19" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="B143" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B143" s="19" t="s">
-        <v>401</v>
-      </c>
       <c r="C143" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D143" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E143" s="20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F143" s="19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="B144" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B144" s="19" t="s">
-        <v>401</v>
-      </c>
       <c r="C144" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D144" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E144" s="20" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F144" s="19" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B145" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="C145" t="s">
+        <v>405</v>
+      </c>
+      <c r="D145" t="s">
         <v>406</v>
       </c>
-      <c r="C145" t="s">
-        <v>406</v>
-      </c>
-      <c r="D145" t="s">
-        <v>407</v>
-      </c>
       <c r="E145" s="20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F145" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B146" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C146" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D146" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E146" s="20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F146" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B147" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C147" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D147" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E147" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F147" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B148" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C148" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D148" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E148" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F148" s="19" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B149" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C149" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D149" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E149" s="20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F149" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B150" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C150" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D150" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E150" s="20" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F150" s="19" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B151" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="C151" t="s">
+        <v>412</v>
+      </c>
+      <c r="D151" t="s">
         <v>413</v>
       </c>
-      <c r="C151" t="s">
-        <v>413</v>
-      </c>
-      <c r="D151" t="s">
-        <v>414</v>
-      </c>
       <c r="E151" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F151" s="19" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B152" s="19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C152" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D152" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E152" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F152" s="19" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B153" s="19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C153" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D153" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E153" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F153" s="19" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B154" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="C154" t="s">
+        <v>416</v>
+      </c>
+      <c r="D154" t="s">
         <v>417</v>
       </c>
-      <c r="C154" t="s">
-        <v>417</v>
-      </c>
-      <c r="D154" t="s">
-        <v>418</v>
-      </c>
       <c r="E154" s="20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F154" s="19" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B155" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C155" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D155" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E155" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F155" s="19" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B156" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C156" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D156" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E156" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F156" s="19" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B157" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C157" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D157" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E157" s="20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F157" s="19" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B158" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C158" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D158" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E158" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F158" s="19" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B159" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C159" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D159" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E159" s="20" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F159" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B160" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C160" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D160" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E160" s="20" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F160" s="19" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B161" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C161" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D161" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E161" s="20" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F161" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B162" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C162" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D162" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E162" s="20" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F162" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B163" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C163" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D163" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E163" s="20" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F163" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B164" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C164" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D164" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E164" s="20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F164" s="19" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B165" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C165" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D165" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E165" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F165" s="19" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B166" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C166" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D166" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E166" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F166" s="19" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B167" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C167" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D167" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E167" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F167" s="19" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B168" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C168" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D168" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E168" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F168" s="19" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B169" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C169" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D169" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E169" s="20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F169" s="19" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B170" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C170" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D170" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E170" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F170" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B171" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C171" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D171" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E171" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F171" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B172" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C172" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D172" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E172" s="20" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F172" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B173" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C173" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D173" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E173" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F173" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B174" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C174" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D174" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E174" s="20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F174" s="19" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B175" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C175" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D175" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E175" s="20" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F175" s="19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B176" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C176" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D176" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E176" s="20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F176" s="19" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B177" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C177" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D177" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E177" s="20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F177" s="19" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B178" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C178" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D178" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E178" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F178" s="19" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B179" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C179" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D179" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E179" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F179" s="19" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B180" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C180" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D180" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E180" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F180" s="19" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B181" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C181" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D181" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E181" s="20" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B182" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C182" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D182" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E182" s="20" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F182" s="19" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B183" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C183" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D183" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E183" s="20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B184" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="C184" t="s">
+        <v>447</v>
+      </c>
+      <c r="D184" t="s">
         <v>448</v>
       </c>
-      <c r="C184" t="s">
-        <v>448</v>
-      </c>
-      <c r="D184" t="s">
-        <v>449</v>
-      </c>
       <c r="E184" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F184" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B185" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C185" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D185" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E185" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F185" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B186" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C186" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D186" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E186" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F186" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B187" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C187" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D187" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E187" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F187" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B188" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C188" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D188" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E188" s="20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F188" s="19" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B189" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C189" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D189" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E189" s="20" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F189" s="19" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B190" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C190" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D190" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E190" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F190" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B191" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C191" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D191" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E191" s="20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F191" s="19" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B192" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C192" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D192" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E192" s="20" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F192" s="19" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B193" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C193" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D193" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E193" s="20" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F193" s="19" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B194" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C194" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D194" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E194" s="20" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F194" s="19" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B195" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C195" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D195" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E195" s="20" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F195" s="19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B196" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C196" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D196" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E196" s="20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F196" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B197" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C197" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D197" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E197" s="20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F197" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B198" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C198" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D198" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E198" s="20" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F198" s="19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B199" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C199" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D199" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E199" s="20" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F199" s="19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B200" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C200" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D200" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E200" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F200" s="19" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B201" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="C201" t="s">
+        <v>465</v>
+      </c>
+      <c r="D201" t="s">
         <v>466</v>
       </c>
-      <c r="C201" t="s">
-        <v>466</v>
-      </c>
-      <c r="D201" t="s">
-        <v>467</v>
-      </c>
       <c r="E201" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F201" s="19" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B202" s="19" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C202" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D202" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E202" s="20" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F202" s="19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B203" s="19" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C203" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D203" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E203" s="20" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F203" s="19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B204" s="19" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C204" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D204" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E204" s="20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F204" s="19" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B205" s="19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C205" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D205" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E205" s="20" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F205" s="19" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B206" s="19" t="s">
+        <v>471</v>
+      </c>
+      <c r="C206" t="s">
+        <v>471</v>
+      </c>
+      <c r="D206" t="s">
         <v>472</v>
       </c>
-      <c r="C206" t="s">
-        <v>472</v>
-      </c>
-      <c r="D206" t="s">
-        <v>473</v>
-      </c>
       <c r="E206" s="20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F206" s="19" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" s="25" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="B207" s="25" t="s">
         <v>15</v>
@@ -6632,18 +6626,18 @@
         <v>22</v>
       </c>
       <c r="D207" s="23" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E207" s="24" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F207" s="17" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" s="25" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="B208" s="25" t="s">
         <v>15</v>
@@ -6652,18 +6646,18 @@
         <v>22</v>
       </c>
       <c r="D208" s="23" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E208" s="24" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F208" s="18" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209" s="25" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="B209" s="25" t="s">
         <v>15</v>
@@ -6672,18 +6666,18 @@
         <v>22</v>
       </c>
       <c r="D209" s="23" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E209" s="24" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F209" s="18" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A210" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B210" s="25" t="s">
         <v>15</v>
@@ -6692,18 +6686,18 @@
         <v>22</v>
       </c>
       <c r="D210" s="23" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E210" s="24" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F210" s="18" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A211" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B211" s="25" t="s">
         <v>15</v>
@@ -6712,18 +6706,18 @@
         <v>22</v>
       </c>
       <c r="D211" s="23" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E211" s="24" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F211" s="18" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A212" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B212" s="25" t="s">
         <v>15</v>
@@ -6732,257 +6726,257 @@
         <v>22</v>
       </c>
       <c r="D212" s="23" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E212" s="24" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F212" s="18" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A213" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B213" s="25" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C213" s="25" t="s">
         <v>22</v>
       </c>
       <c r="D213" s="23" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E213" s="24" t="s">
         <v>262</v>
       </c>
       <c r="F213" s="18" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A214" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B214" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="C214" s="25" t="s">
         <v>576</v>
       </c>
-      <c r="C214" s="25" t="s">
+      <c r="D214" s="23" t="s">
+        <v>577</v>
+      </c>
+      <c r="E214" s="24" t="s">
         <v>578</v>
       </c>
-      <c r="D214" s="23" t="s">
-        <v>579</v>
-      </c>
-      <c r="E214" s="24" t="s">
-        <v>580</v>
-      </c>
       <c r="F214" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="215" spans="1:6" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A215" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B215" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="C215" s="25" t="s">
         <v>576</v>
       </c>
-      <c r="C215" s="25" t="s">
-        <v>578</v>
-      </c>
       <c r="D215" s="23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E215" s="24" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F215" s="26" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="216" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A216" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B216" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="C216" s="25" t="s">
         <v>576</v>
       </c>
-      <c r="C216" s="25" t="s">
-        <v>578</v>
-      </c>
       <c r="D216" s="23" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E216" s="24" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F216" s="18" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="217" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A217" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B217" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="C217" s="25" t="s">
         <v>576</v>
       </c>
-      <c r="C217" s="25" t="s">
-        <v>578</v>
-      </c>
       <c r="D217" s="25" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E217" s="24" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F217" s="18" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="218" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A218" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B218" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="C218" s="25" t="s">
         <v>576</v>
       </c>
-      <c r="C218" s="25" t="s">
-        <v>578</v>
-      </c>
       <c r="D218" s="25" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E218" s="24" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F218" s="18" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="219" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A219" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B219" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="C219" s="25" t="s">
         <v>576</v>
       </c>
-      <c r="C219" s="25" t="s">
-        <v>578</v>
-      </c>
       <c r="D219" s="25" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E219" s="24" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F219" s="18" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="220" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A220" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B220" s="25" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C220" s="25" t="s">
+        <v>585</v>
+      </c>
+      <c r="D220" s="23" t="s">
+        <v>586</v>
+      </c>
+      <c r="E220" s="24" t="s">
         <v>587</v>
       </c>
-      <c r="D220" s="23" t="s">
-        <v>588</v>
-      </c>
-      <c r="E220" s="24" t="s">
-        <v>589</v>
-      </c>
       <c r="F220" s="18" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A221" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B221" s="25" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C221" s="25" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D221" s="23" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E221" s="24" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F221" s="18" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="222" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A222" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B222" s="25" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C222" s="25" t="s">
+        <v>590</v>
+      </c>
+      <c r="D222" s="23" t="s">
+        <v>591</v>
+      </c>
+      <c r="E222" s="24" t="s">
         <v>592</v>
       </c>
-      <c r="D222" s="23" t="s">
-        <v>593</v>
-      </c>
-      <c r="E222" s="24" t="s">
-        <v>594</v>
-      </c>
       <c r="F222" s="18" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="223" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A223" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B223" s="25" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C223" s="25" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D223" s="23" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E223" s="24" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F223" s="18" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A224" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B224" s="25" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C224" s="25" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D224" s="25" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E224" s="24" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F224" s="18" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G111" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}"/>
+  <autoFilter ref="A1:G224" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}"/>
   <hyperlinks>
     <hyperlink ref="L11" r:id="rId1" display="https://teams.mdlz.com/:b:/r/sites/dadocumentrepository/Shared Documents/Data Domain Experts/DaaS PPTs/May 2024 Visit Final versions/DaaS Day in life - Functional Towers.pdf?csf=1&amp;web=1&amp;e=b3v3fi" xr:uid="{C9234C41-0B35-449D-A059-14FCD43DD586}"/>
     <hyperlink ref="L12" r:id="rId2" display="https://collaboration.mdlz.com/sites/daas/SitePages/DA_DDD.aspx" xr:uid="{B1E49C27-813B-4F81-B6D4-F88CC7C95F9A}"/>
@@ -7363,7 +7357,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>140</v>
@@ -7374,7 +7368,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>185</v>
@@ -7385,7 +7379,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>284</v>
@@ -7396,7 +7390,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>140</v>
@@ -7407,7 +7401,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>141</v>
@@ -7418,7 +7412,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>154</v>
@@ -7429,7 +7423,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>139</v>
@@ -7440,7 +7434,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>283</v>
@@ -7451,7 +7445,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
Added CAB checklist & D&A onboarding package
</commit_message>
<xml_diff>
--- a/data/chatbot-1.xlsx
+++ b/data/chatbot-1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJK3794\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AC0144-D16C-4739-A11E-431B113F110B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8499C1-BD2B-424A-952D-B006BE8CB358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CB1DE796-0A7F-4358-B0F5-62D7433C0693}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FAQ!$A$1:$A$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$225</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$226</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentManualCount="16"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="630">
   <si>
     <t>Category</t>
   </si>
@@ -1908,6 +1908,30 @@
   </si>
   <si>
     <t>https://collaboration.mdlz.com/sites/daas/Shared%20Documents/Forms/AllItems.aspx?id=%2Fsites%2Fdaas%2FShared%20Documents%2FData%20COE%20WoW%2FData%20COE%20End%2Dto%2DEnd%20Process%20Document%2Epdf&amp;parent=%2Fsites%2Fdaas%2FShared%20Documents%2FData%20COE%20WoW&amp;p=true&amp;ga=1</t>
+  </si>
+  <si>
+    <t>Where can I find the document that will provide new suppliers, contractors, and internal new Mondelez employees with information about the setup of the Data and Analytics organization, the multiple teams involved in transforming data into information, as well as the policies, procedures, and standards established within the Mondelez Data and Analytics organization?</t>
+  </si>
+  <si>
+    <t>D&amp;A Onboarding Package</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/:w:/r/sites/dataandanalyticsgrowprogram/Shared%20Documents/Onboarding/D%26A%20Onboarding%20Package.docx?d=wffb7ff4307d44e199e81c2ce25dfc252&amp;csf=1&amp;web=1&amp;e=U81Fw5</t>
+  </si>
+  <si>
+    <t>D4GV</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Where can I find the check list for CAB review?</t>
+  </si>
+  <si>
+    <t>D4GV CAB Check List.xlsx</t>
+  </si>
+  <si>
+    <t>https://teams.mdlz.com/:x:/r/sites/ibsdataandanalytics/Shared%20Documents/D%26A%20Calendar/D4GV%20CAB%20Check%20List.xlsx?d=wa29ba62f00ba4fb1921700f2de347e92&amp;csf=1&amp;web=1&amp;e=zXLJvY</t>
   </si>
 </sst>
 </file>
@@ -2007,7 +2031,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2061,6 +2085,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2376,11 +2403,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}">
-  <dimension ref="A1:L225"/>
+  <dimension ref="A1:L227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="E229" sqref="E229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6767,27 +6794,27 @@
         <v>606</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:6" s="22" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A214" s="25" t="s">
         <v>567</v>
       </c>
       <c r="B214" s="25" t="s">
-        <v>574</v>
+        <v>15</v>
       </c>
       <c r="C214" s="25" t="s">
         <v>22</v>
       </c>
       <c r="D214" s="23" t="s">
-        <v>575</v>
+        <v>622</v>
       </c>
       <c r="E214" s="24" t="s">
-        <v>262</v>
+        <v>624</v>
       </c>
       <c r="F214" s="18" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A215" s="25" t="s">
         <v>567</v>
       </c>
@@ -6795,19 +6822,19 @@
         <v>574</v>
       </c>
       <c r="C215" s="25" t="s">
-        <v>576</v>
+        <v>22</v>
       </c>
       <c r="D215" s="23" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E215" s="24" t="s">
-        <v>578</v>
-      </c>
-      <c r="F215" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>262</v>
+      </c>
+      <c r="F215" s="18" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A216" s="25" t="s">
         <v>567</v>
       </c>
@@ -6818,16 +6845,16 @@
         <v>576</v>
       </c>
       <c r="D216" s="23" t="s">
-        <v>597</v>
+        <v>577</v>
       </c>
       <c r="E216" s="24" t="s">
-        <v>598</v>
-      </c>
-      <c r="F216" s="26" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>578</v>
+      </c>
+      <c r="F216" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A217" s="25" t="s">
         <v>567</v>
       </c>
@@ -6838,16 +6865,16 @@
         <v>576</v>
       </c>
       <c r="D217" s="23" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E217" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="F217" s="18" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>598</v>
+      </c>
+      <c r="F217" s="26" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A218" s="25" t="s">
         <v>567</v>
       </c>
@@ -6857,17 +6884,17 @@
       <c r="C218" s="25" t="s">
         <v>576</v>
       </c>
-      <c r="D218" s="25" t="s">
-        <v>579</v>
+      <c r="D218" s="23" t="s">
+        <v>600</v>
       </c>
       <c r="E218" s="24" t="s">
-        <v>580</v>
+        <v>599</v>
       </c>
       <c r="F218" s="18" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A219" s="25" t="s">
         <v>567</v>
       </c>
@@ -6878,13 +6905,13 @@
         <v>576</v>
       </c>
       <c r="D219" s="25" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E219" s="24" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F219" s="18" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="220" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -6898,13 +6925,13 @@
         <v>576</v>
       </c>
       <c r="D220" s="25" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E220" s="24" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F220" s="18" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -6915,19 +6942,19 @@
         <v>574</v>
       </c>
       <c r="C221" s="25" t="s">
-        <v>585</v>
-      </c>
-      <c r="D221" s="23" t="s">
-        <v>586</v>
+        <v>576</v>
+      </c>
+      <c r="D221" s="25" t="s">
+        <v>583</v>
       </c>
       <c r="E221" s="24" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="F221" s="18" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A222" s="25" t="s">
         <v>567</v>
       </c>
@@ -6938,16 +6965,16 @@
         <v>585</v>
       </c>
       <c r="D222" s="23" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E222" s="24" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F222" s="18" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A223" s="25" t="s">
         <v>567</v>
       </c>
@@ -6955,16 +6982,16 @@
         <v>574</v>
       </c>
       <c r="C223" s="25" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="D223" s="23" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E223" s="24" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F223" s="18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -6978,13 +7005,13 @@
         <v>590</v>
       </c>
       <c r="D224" s="23" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E224" s="24" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F224" s="18" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="225" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -6997,18 +7024,58 @@
       <c r="C225" s="25" t="s">
         <v>590</v>
       </c>
-      <c r="D225" s="25" t="s">
+      <c r="D225" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="E225" s="24" t="s">
+        <v>594</v>
+      </c>
+      <c r="F225" s="18" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A226" s="25" t="s">
+        <v>567</v>
+      </c>
+      <c r="B226" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="C226" s="25" t="s">
+        <v>590</v>
+      </c>
+      <c r="D226" s="25" t="s">
         <v>595</v>
       </c>
-      <c r="E225" s="24" t="s">
+      <c r="E226" s="24" t="s">
         <v>596</v>
       </c>
-      <c r="F225" s="18" t="s">
+      <c r="F226" s="18" t="s">
         <v>618</v>
       </c>
     </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A227" s="26" t="s">
+        <v>625</v>
+      </c>
+      <c r="B227" s="26" t="s">
+        <v>574</v>
+      </c>
+      <c r="C227" s="26" t="s">
+        <v>626</v>
+      </c>
+      <c r="D227" s="27" t="s">
+        <v>627</v>
+      </c>
+      <c r="E227" s="24" t="s">
+        <v>629</v>
+      </c>
+      <c r="F227" s="20" t="s">
+        <v>628</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G225" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}"/>
+  <autoFilter ref="A1:G226" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}"/>
   <hyperlinks>
     <hyperlink ref="L11" r:id="rId1" display="https://teams.mdlz.com/:b:/r/sites/dadocumentrepository/Shared Documents/Data Domain Experts/DaaS PPTs/May 2024 Visit Final versions/DaaS Day in life - Functional Towers.pdf?csf=1&amp;web=1&amp;e=b3v3fi" xr:uid="{C9234C41-0B35-449D-A059-14FCD43DD586}"/>
     <hyperlink ref="L13" r:id="rId2" display="https://collaboration.mdlz.com/sites/daas/SitePages/DA_DDD.aspx" xr:uid="{B1E49C27-813B-4F81-B6D4-F88CC7C95F9A}"/>
@@ -7341,17 +7408,17 @@
     <hyperlink ref="E211" r:id="rId329" xr:uid="{AF6C72DF-4FBD-4CB0-9D30-4F887C820BC6}"/>
     <hyperlink ref="E212" r:id="rId330" xr:uid="{B5DB5909-CAE3-41DE-8FAA-2BE9405FE89D}"/>
     <hyperlink ref="E213" r:id="rId331" xr:uid="{EB971EED-5319-4B5A-866B-6272F1177031}"/>
-    <hyperlink ref="E214" r:id="rId332" xr:uid="{572B6EAD-FA78-4215-8917-A3C00D5ABFE0}"/>
-    <hyperlink ref="E215" r:id="rId333" display="https://teams.mdlz.com/sites/enterprisedataplatformteam/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=C7C4X1&amp;CID=8d0e24a9%2D7bea%2D46a6%2D9501%2D656778853926&amp;FolderCTID=0x012000C3AAEF24304CAA4B9AE73A9B852BAD69&amp;id=%2Fsites%2Fenterprisedataplatformteam%2FShared%20Documents%2FGeneral%2FD%26A%5FGovernance%20%26%20Methodology%2F1%2E%20D%26A%20Operating%20Model" xr:uid="{68BBCE6F-8DA7-464D-950F-BC16B0FF571C}"/>
-    <hyperlink ref="E221" r:id="rId334" xr:uid="{4CB97E97-7749-4435-94AD-D2868D458F68}"/>
-    <hyperlink ref="E223" r:id="rId335" xr:uid="{A474367E-A77D-4DEF-85B7-EEA70951388E}"/>
-    <hyperlink ref="E224" r:id="rId336" xr:uid="{68A144C1-9301-4982-9D52-3E933824C145}"/>
-    <hyperlink ref="E225" r:id="rId337" xr:uid="{A289F92F-FDC4-4101-860D-E87FC724D2BF}"/>
-    <hyperlink ref="E218" r:id="rId338" xr:uid="{7FE505FE-5854-4EEC-9F18-EC57B446CAB8}"/>
-    <hyperlink ref="E219" r:id="rId339" xr:uid="{FAF735B2-76DF-4822-819D-3825B225638C}"/>
-    <hyperlink ref="E220" r:id="rId340" xr:uid="{BFCB53CB-917E-4F45-9B9B-5CF694A05B23}"/>
-    <hyperlink ref="E222" r:id="rId341" xr:uid="{60C77EDA-E2FD-4625-89AC-626B3B109939}"/>
-    <hyperlink ref="E217" r:id="rId342" xr:uid="{9B7F4E7B-88C8-478A-BA8C-0835ECDAC49D}"/>
+    <hyperlink ref="E215" r:id="rId332" xr:uid="{572B6EAD-FA78-4215-8917-A3C00D5ABFE0}"/>
+    <hyperlink ref="E216" r:id="rId333" display="https://teams.mdlz.com/sites/enterprisedataplatformteam/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=C7C4X1&amp;CID=8d0e24a9%2D7bea%2D46a6%2D9501%2D656778853926&amp;FolderCTID=0x012000C3AAEF24304CAA4B9AE73A9B852BAD69&amp;id=%2Fsites%2Fenterprisedataplatformteam%2FShared%20Documents%2FGeneral%2FD%26A%5FGovernance%20%26%20Methodology%2F1%2E%20D%26A%20Operating%20Model" xr:uid="{68BBCE6F-8DA7-464D-950F-BC16B0FF571C}"/>
+    <hyperlink ref="E222" r:id="rId334" xr:uid="{4CB97E97-7749-4435-94AD-D2868D458F68}"/>
+    <hyperlink ref="E224" r:id="rId335" xr:uid="{A474367E-A77D-4DEF-85B7-EEA70951388E}"/>
+    <hyperlink ref="E225" r:id="rId336" xr:uid="{68A144C1-9301-4982-9D52-3E933824C145}"/>
+    <hyperlink ref="E226" r:id="rId337" xr:uid="{A289F92F-FDC4-4101-860D-E87FC724D2BF}"/>
+    <hyperlink ref="E219" r:id="rId338" xr:uid="{7FE505FE-5854-4EEC-9F18-EC57B446CAB8}"/>
+    <hyperlink ref="E220" r:id="rId339" xr:uid="{FAF735B2-76DF-4822-819D-3825B225638C}"/>
+    <hyperlink ref="E221" r:id="rId340" xr:uid="{BFCB53CB-917E-4F45-9B9B-5CF694A05B23}"/>
+    <hyperlink ref="E223" r:id="rId341" xr:uid="{60C77EDA-E2FD-4625-89AC-626B3B109939}"/>
+    <hyperlink ref="E218" r:id="rId342" xr:uid="{9B7F4E7B-88C8-478A-BA8C-0835ECDAC49D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId343"/>

</xml_diff>

<commit_message>
changed category for cab checklist
</commit_message>
<xml_diff>
--- a/data/chatbot-1.xlsx
+++ b/data/chatbot-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJK3794\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8499C1-BD2B-424A-952D-B006BE8CB358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5E41CA-88D6-4B66-ABAB-F950C20B84D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CB1DE796-0A7F-4358-B0F5-62D7433C0693}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FAQ!$A$1:$A$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$226</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$227</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentManualCount="16"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="629">
   <si>
     <t>Category</t>
   </si>
@@ -1917,9 +1917,6 @@
   </si>
   <si>
     <t>https://teams.mdlz.com/:w:/r/sites/dataandanalyticsgrowprogram/Shared%20Documents/Onboarding/D%26A%20Onboarding%20Package.docx?d=wffb7ff4307d44e199e81c2ce25dfc252&amp;csf=1&amp;web=1&amp;e=U81Fw5</t>
-  </si>
-  <si>
-    <t>D4GV</t>
   </si>
   <si>
     <t>Project Management</t>
@@ -2406,8 +2403,8 @@
   <dimension ref="A1:L227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E229" sqref="E229"/>
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A227" sqref="A227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7054,28 +7051,28 @@
         <v>618</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A227" s="26" t="s">
-        <v>625</v>
+    <row r="227" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A227" s="25" t="s">
+        <v>567</v>
       </c>
       <c r="B227" s="26" t="s">
         <v>574</v>
       </c>
       <c r="C227" s="26" t="s">
+        <v>625</v>
+      </c>
+      <c r="D227" s="27" t="s">
         <v>626</v>
       </c>
-      <c r="D227" s="27" t="s">
+      <c r="E227" s="24" t="s">
+        <v>628</v>
+      </c>
+      <c r="F227" s="20" t="s">
         <v>627</v>
       </c>
-      <c r="E227" s="24" t="s">
-        <v>629</v>
-      </c>
-      <c r="F227" s="20" t="s">
-        <v>628</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G226" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}"/>
+  <autoFilter ref="A1:G227" xr:uid="{7EA498B8-987A-47B6-87ED-78E5DE62CE2C}"/>
   <hyperlinks>
     <hyperlink ref="L11" r:id="rId1" display="https://teams.mdlz.com/:b:/r/sites/dadocumentrepository/Shared Documents/Data Domain Experts/DaaS PPTs/May 2024 Visit Final versions/DaaS Day in life - Functional Towers.pdf?csf=1&amp;web=1&amp;e=b3v3fi" xr:uid="{C9234C41-0B35-449D-A059-14FCD43DD586}"/>
     <hyperlink ref="L13" r:id="rId2" display="https://collaboration.mdlz.com/sites/daas/SitePages/DA_DDD.aspx" xr:uid="{B1E49C27-813B-4F81-B6D4-F88CC7C95F9A}"/>

</xml_diff>